<commit_message>
Atualizado por script em 10-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/bulgaria_vtora-liga_2023-2024.xlsx
+++ b/2023/bulgaria_vtora-liga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V142"/>
+  <dimension ref="A1:V143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11981,22 +11981,22 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Ludogorets II</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="G126" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Belasitsa</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="I126" t="n">
         <v>1</v>
       </c>
       <c r="J126" t="n">
-        <v>1.68</v>
+        <v>2</v>
       </c>
       <c r="K126" t="inlineStr">
         <is>
@@ -12004,15 +12004,15 @@
         </is>
       </c>
       <c r="L126" t="n">
-        <v>1.6</v>
+        <v>1.85</v>
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>27/10/2023 13:03</t>
+          <t>27/10/2023 14:48</t>
         </is>
       </c>
       <c r="N126" t="n">
-        <v>3.24</v>
+        <v>2.86</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -12020,15 +12020,15 @@
         </is>
       </c>
       <c r="P126" t="n">
-        <v>3.51</v>
+        <v>2.88</v>
       </c>
       <c r="Q126" t="inlineStr">
         <is>
-          <t>27/10/2023 13:41</t>
+          <t>27/10/2023 14:48</t>
         </is>
       </c>
       <c r="R126" t="n">
-        <v>4.05</v>
+        <v>3.34</v>
       </c>
       <c r="S126" t="inlineStr">
         <is>
@@ -12036,16 +12036,16 @@
         </is>
       </c>
       <c r="T126" t="n">
-        <v>5.13</v>
+        <v>4.6</v>
       </c>
       <c r="U126" t="inlineStr">
         <is>
-          <t>27/10/2023 13:03</t>
+          <t>27/10/2023 14:48</t>
         </is>
       </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-belasitsa-petrich/xt6eoi3l/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-dunav-ruse/4lkJ4u49/</t>
         </is>
       </c>
     </row>
@@ -12625,22 +12625,22 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Ludogorets II</t>
         </is>
       </c>
       <c r="G133" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Belasitsa</t>
         </is>
       </c>
       <c r="I133" t="n">
         <v>1</v>
       </c>
       <c r="J133" t="n">
-        <v>2</v>
+        <v>1.68</v>
       </c>
       <c r="K133" t="inlineStr">
         <is>
@@ -12648,15 +12648,15 @@
         </is>
       </c>
       <c r="L133" t="n">
-        <v>1.85</v>
+        <v>1.6</v>
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>27/10/2023 14:48</t>
+          <t>27/10/2023 13:03</t>
         </is>
       </c>
       <c r="N133" t="n">
-        <v>2.86</v>
+        <v>3.24</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -12664,15 +12664,15 @@
         </is>
       </c>
       <c r="P133" t="n">
-        <v>2.88</v>
+        <v>3.51</v>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>27/10/2023 14:48</t>
+          <t>27/10/2023 13:41</t>
         </is>
       </c>
       <c r="R133" t="n">
-        <v>3.34</v>
+        <v>4.05</v>
       </c>
       <c r="S133" t="inlineStr">
         <is>
@@ -12680,16 +12680,16 @@
         </is>
       </c>
       <c r="T133" t="n">
-        <v>4.6</v>
+        <v>5.13</v>
       </c>
       <c r="U133" t="inlineStr">
         <is>
-          <t>27/10/2023 14:48</t>
+          <t>27/10/2023 13:03</t>
         </is>
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-dunav-ruse/4lkJ4u49/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-belasitsa-petrich/xt6eoi3l/</t>
         </is>
       </c>
     </row>
@@ -12717,7 +12717,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="G134" t="n">
@@ -12725,14 +12725,14 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Yantra Gabrovo</t>
+          <t>CSKA 1948 Sofia II</t>
         </is>
       </c>
       <c r="I134" t="n">
         <v>1</v>
       </c>
       <c r="J134" t="n">
-        <v>2.15</v>
+        <v>4.31</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -12740,15 +12740,15 @@
         </is>
       </c>
       <c r="L134" t="n">
-        <v>2.42</v>
+        <v>4.54</v>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>03/11/2023 12:25</t>
+          <t>03/11/2023 13:23</t>
         </is>
       </c>
       <c r="N134" t="n">
-        <v>2.79</v>
+        <v>3.15</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -12756,15 +12756,15 @@
         </is>
       </c>
       <c r="P134" t="n">
-        <v>2.78</v>
+        <v>2.8</v>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>03/11/2023 12:25</t>
+          <t>03/11/2023 13:23</t>
         </is>
       </c>
       <c r="R134" t="n">
-        <v>3.09</v>
+        <v>1.67</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -12772,16 +12772,16 @@
         </is>
       </c>
       <c r="T134" t="n">
-        <v>3.01</v>
+        <v>1.89</v>
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>03/11/2023 12:25</t>
+          <t>03/11/2023 13:23</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-yantra-gabrovo/6LcCs92D/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-cska-1948-sofia/Wbkb5CfK/</t>
         </is>
       </c>
     </row>
@@ -12809,22 +12809,22 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Belasitsa</t>
         </is>
       </c>
       <c r="G135" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>CSKA 1948 Sofia II</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="I135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J135" t="n">
-        <v>4.31</v>
+        <v>1.94</v>
       </c>
       <c r="K135" t="inlineStr">
         <is>
@@ -12832,15 +12832,15 @@
         </is>
       </c>
       <c r="L135" t="n">
-        <v>4.54</v>
+        <v>1.64</v>
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>03/11/2023 13:23</t>
+          <t>03/11/2023 13:29</t>
         </is>
       </c>
       <c r="N135" t="n">
-        <v>3.15</v>
+        <v>2.98</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -12848,15 +12848,15 @@
         </is>
       </c>
       <c r="P135" t="n">
-        <v>2.8</v>
+        <v>3.49</v>
       </c>
       <c r="Q135" t="inlineStr">
         <is>
-          <t>03/11/2023 13:23</t>
+          <t>03/11/2023 13:29</t>
         </is>
       </c>
       <c r="R135" t="n">
-        <v>1.67</v>
+        <v>3.35</v>
       </c>
       <c r="S135" t="inlineStr">
         <is>
@@ -12864,16 +12864,16 @@
         </is>
       </c>
       <c r="T135" t="n">
-        <v>1.89</v>
+        <v>4.74</v>
       </c>
       <c r="U135" t="inlineStr">
         <is>
-          <t>03/11/2023 13:23</t>
+          <t>03/11/2023 13:29</t>
         </is>
       </c>
       <c r="V135" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-cska-1948-sofia/Wbkb5CfK/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/belasitsa-petrich-spartak-pleven/ENv34W9Q/</t>
         </is>
       </c>
     </row>
@@ -12901,22 +12901,22 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Belasitsa</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="G136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="I136" t="n">
         <v>2</v>
       </c>
       <c r="J136" t="n">
-        <v>1.94</v>
+        <v>1.91</v>
       </c>
       <c r="K136" t="inlineStr">
         <is>
@@ -12924,15 +12924,15 @@
         </is>
       </c>
       <c r="L136" t="n">
-        <v>1.64</v>
+        <v>1.72</v>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>03/11/2023 13:29</t>
+          <t>03/11/2023 13:26</t>
         </is>
       </c>
       <c r="N136" t="n">
-        <v>2.98</v>
+        <v>2.97</v>
       </c>
       <c r="O136" t="inlineStr">
         <is>
@@ -12940,15 +12940,15 @@
         </is>
       </c>
       <c r="P136" t="n">
-        <v>3.49</v>
+        <v>3.23</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
-          <t>03/11/2023 13:29</t>
+          <t>03/11/2023 13:26</t>
         </is>
       </c>
       <c r="R136" t="n">
-        <v>3.35</v>
+        <v>3.48</v>
       </c>
       <c r="S136" t="inlineStr">
         <is>
@@ -12956,16 +12956,16 @@
         </is>
       </c>
       <c r="T136" t="n">
-        <v>4.74</v>
+        <v>4.67</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>03/11/2023 13:29</t>
+          <t>03/11/2023 12:47</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/belasitsa-petrich-spartak-pleven/ENv34W9Q/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-1919-svoge/KOof6huE/</t>
         </is>
       </c>
     </row>
@@ -12993,22 +12993,22 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="G137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="I137" t="n">
         <v>2</v>
       </c>
       <c r="J137" t="n">
-        <v>1.91</v>
+        <v>1.36</v>
       </c>
       <c r="K137" t="inlineStr">
         <is>
@@ -13016,15 +13016,15 @@
         </is>
       </c>
       <c r="L137" t="n">
-        <v>1.72</v>
+        <v>1.37</v>
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>03/11/2023 13:26</t>
+          <t>03/11/2023 12:42</t>
         </is>
       </c>
       <c r="N137" t="n">
-        <v>2.97</v>
+        <v>3.94</v>
       </c>
       <c r="O137" t="inlineStr">
         <is>
@@ -13032,15 +13032,15 @@
         </is>
       </c>
       <c r="P137" t="n">
-        <v>3.23</v>
+        <v>4.03</v>
       </c>
       <c r="Q137" t="inlineStr">
         <is>
-          <t>03/11/2023 13:26</t>
+          <t>03/11/2023 13:18</t>
         </is>
       </c>
       <c r="R137" t="n">
-        <v>3.48</v>
+        <v>6.19</v>
       </c>
       <c r="S137" t="inlineStr">
         <is>
@@ -13048,16 +13048,16 @@
         </is>
       </c>
       <c r="T137" t="n">
-        <v>4.67</v>
+        <v>8.08</v>
       </c>
       <c r="U137" t="inlineStr">
         <is>
-          <t>03/11/2023 12:47</t>
+          <t>03/11/2023 13:18</t>
         </is>
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-1919-svoge/KOof6huE/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-strumska-slava/KONod8H6/</t>
         </is>
       </c>
     </row>
@@ -13085,22 +13085,22 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="G138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Yantra Gabrovo</t>
         </is>
       </c>
       <c r="I138" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J138" t="n">
-        <v>1.36</v>
+        <v>2.15</v>
       </c>
       <c r="K138" t="inlineStr">
         <is>
@@ -13108,15 +13108,15 @@
         </is>
       </c>
       <c r="L138" t="n">
-        <v>1.37</v>
+        <v>2.42</v>
       </c>
       <c r="M138" t="inlineStr">
         <is>
-          <t>03/11/2023 12:42</t>
+          <t>03/11/2023 12:25</t>
         </is>
       </c>
       <c r="N138" t="n">
-        <v>3.94</v>
+        <v>2.79</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -13124,15 +13124,15 @@
         </is>
       </c>
       <c r="P138" t="n">
-        <v>4.03</v>
+        <v>2.78</v>
       </c>
       <c r="Q138" t="inlineStr">
         <is>
-          <t>03/11/2023 13:18</t>
+          <t>03/11/2023 12:25</t>
         </is>
       </c>
       <c r="R138" t="n">
-        <v>6.19</v>
+        <v>3.09</v>
       </c>
       <c r="S138" t="inlineStr">
         <is>
@@ -13140,16 +13140,16 @@
         </is>
       </c>
       <c r="T138" t="n">
-        <v>8.08</v>
+        <v>3.01</v>
       </c>
       <c r="U138" t="inlineStr">
         <is>
-          <t>03/11/2023 13:18</t>
+          <t>03/11/2023 12:25</t>
         </is>
       </c>
       <c r="V138" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-strumska-slava/KONod8H6/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-yantra-gabrovo/6LcCs92D/</t>
         </is>
       </c>
     </row>
@@ -13361,22 +13361,22 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Spartak Varna</t>
         </is>
       </c>
       <c r="G141" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>Litex Lovech</t>
+          <t>Ludogorets II</t>
         </is>
       </c>
       <c r="I141" t="n">
         <v>0</v>
       </c>
       <c r="J141" t="n">
-        <v>2</v>
+        <v>1.38</v>
       </c>
       <c r="K141" t="inlineStr">
         <is>
@@ -13384,15 +13384,15 @@
         </is>
       </c>
       <c r="L141" t="n">
-        <v>2.01</v>
+        <v>1.22</v>
       </c>
       <c r="M141" t="inlineStr">
         <is>
-          <t>07/11/2023 13:28</t>
+          <t>07/11/2023 13:26</t>
         </is>
       </c>
       <c r="N141" t="n">
-        <v>3.08</v>
+        <v>4.19</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -13400,15 +13400,15 @@
         </is>
       </c>
       <c r="P141" t="n">
-        <v>3.13</v>
+        <v>5.28</v>
       </c>
       <c r="Q141" t="inlineStr">
         <is>
-          <t>07/11/2023 13:28</t>
+          <t>07/11/2023 13:26</t>
         </is>
       </c>
       <c r="R141" t="n">
-        <v>3.37</v>
+        <v>6.34</v>
       </c>
       <c r="S141" t="inlineStr">
         <is>
@@ -13416,16 +13416,16 @@
         </is>
       </c>
       <c r="T141" t="n">
-        <v>3.47</v>
+        <v>10.71</v>
       </c>
       <c r="U141" t="inlineStr">
         <is>
-          <t>07/11/2023 13:28</t>
+          <t>07/11/2023 13:26</t>
         </is>
       </c>
       <c r="V141" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-litex-lovech/p6VYbAXm/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-varna-ludogorets/GWQUajIs/</t>
         </is>
       </c>
     </row>
@@ -13453,22 +13453,22 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Spartak Varna</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="G142" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>Ludogorets II</t>
+          <t>Litex Lovech</t>
         </is>
       </c>
       <c r="I142" t="n">
         <v>0</v>
       </c>
       <c r="J142" t="n">
-        <v>1.38</v>
+        <v>2</v>
       </c>
       <c r="K142" t="inlineStr">
         <is>
@@ -13476,15 +13476,15 @@
         </is>
       </c>
       <c r="L142" t="n">
-        <v>1.22</v>
+        <v>2.01</v>
       </c>
       <c r="M142" t="inlineStr">
         <is>
-          <t>07/11/2023 13:26</t>
+          <t>07/11/2023 13:28</t>
         </is>
       </c>
       <c r="N142" t="n">
-        <v>4.19</v>
+        <v>3.08</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -13492,15 +13492,15 @@
         </is>
       </c>
       <c r="P142" t="n">
-        <v>5.28</v>
+        <v>3.13</v>
       </c>
       <c r="Q142" t="inlineStr">
         <is>
-          <t>07/11/2023 13:26</t>
+          <t>07/11/2023 13:28</t>
         </is>
       </c>
       <c r="R142" t="n">
-        <v>6.34</v>
+        <v>3.37</v>
       </c>
       <c r="S142" t="inlineStr">
         <is>
@@ -13508,16 +13508,108 @@
         </is>
       </c>
       <c r="T142" t="n">
-        <v>10.71</v>
+        <v>3.47</v>
       </c>
       <c r="U142" t="inlineStr">
         <is>
-          <t>07/11/2023 13:26</t>
+          <t>07/11/2023 13:28</t>
         </is>
       </c>
       <c r="V142" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-varna-ludogorets/GWQUajIs/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-litex-lovech/p6VYbAXm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>bulgaria</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>vtora-liga</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E143" s="2" t="n">
+        <v>45240.5625</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>CSKA 1948 Sofia II</t>
+        </is>
+      </c>
+      <c r="G143" t="n">
+        <v>0</v>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Belasitsa</t>
+        </is>
+      </c>
+      <c r="I143" t="n">
+        <v>0</v>
+      </c>
+      <c r="J143" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>10/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="L143" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>10/11/2023 13:29</t>
+        </is>
+      </c>
+      <c r="N143" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="O143" t="inlineStr">
+        <is>
+          <t>10/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="P143" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="Q143" t="inlineStr">
+        <is>
+          <t>10/11/2023 13:29</t>
+        </is>
+      </c>
+      <c r="R143" t="n">
+        <v>7.38</v>
+      </c>
+      <c r="S143" t="inlineStr">
+        <is>
+          <t>10/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="T143" t="n">
+        <v>6.26</v>
+      </c>
+      <c r="U143" t="inlineStr">
+        <is>
+          <t>10/11/2023 13:29</t>
+        </is>
+      </c>
+      <c r="V143" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/cska-1948-sofia-belasitsa-petrich/pS69BmHg/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 17-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/bulgaria_vtora-liga_2023-2024.xlsx
+++ b/2023/bulgaria_vtora-liga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V151"/>
+  <dimension ref="A1:V152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1861,22 +1861,22 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Ludogorets II</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Septemvri Sofia</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J16" t="n">
-        <v>2.99</v>
+        <v>2.95</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1884,15 +1884,15 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>2.3</v>
+        <v>3.08</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>23/07/2023 17:15</t>
+          <t>23/07/2023 16:11</t>
         </is>
       </c>
       <c r="N16" t="n">
-        <v>3.1</v>
+        <v>3.09</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1900,15 +1900,15 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>3.19</v>
+        <v>3.04</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>23/07/2023 17:15</t>
+          <t>23/07/2023 15:35</t>
         </is>
       </c>
       <c r="R16" t="n">
-        <v>2.2</v>
+        <v>2.23</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
@@ -1916,16 +1916,16 @@
         </is>
       </c>
       <c r="T16" t="n">
-        <v>2.7</v>
+        <v>2.22</v>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>23/07/2023 17:15</t>
+          <t>23/07/2023 16:11</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-montana/U3OY3md1/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-septemvri-sofia/O25PQA3E/</t>
         </is>
       </c>
     </row>
@@ -2045,22 +2045,22 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Ludogorets II</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Septemvri Sofia</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>2.95</v>
+        <v>2.99</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
@@ -2068,15 +2068,15 @@
         </is>
       </c>
       <c r="L18" t="n">
-        <v>3.08</v>
+        <v>2.3</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>23/07/2023 16:11</t>
+          <t>23/07/2023 17:15</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>3.09</v>
+        <v>3.1</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -2084,15 +2084,15 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>3.04</v>
+        <v>3.19</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>23/07/2023 15:35</t>
+          <t>23/07/2023 17:15</t>
         </is>
       </c>
       <c r="R18" t="n">
-        <v>2.23</v>
+        <v>2.2</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
@@ -2100,16 +2100,16 @@
         </is>
       </c>
       <c r="T18" t="n">
-        <v>2.22</v>
+        <v>2.7</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>23/07/2023 16:11</t>
+          <t>23/07/2023 17:15</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-septemvri-sofia/O25PQA3E/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-montana/U3OY3md1/</t>
         </is>
       </c>
     </row>
@@ -9221,22 +9221,22 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Ludogorets II</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="G96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Spartak Varna</t>
         </is>
       </c>
       <c r="I96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J96" t="n">
-        <v>1.88</v>
+        <v>2.15</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
@@ -9244,48 +9244,48 @@
         </is>
       </c>
       <c r="L96" t="n">
-        <v>1.89</v>
+        <v>1.93</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
+          <t>28/09/2023 15:56</t>
+        </is>
+      </c>
+      <c r="N96" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>27/09/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P96" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
           <t>28/09/2023 15:59</t>
         </is>
       </c>
-      <c r="N96" t="n">
-        <v>3.05</v>
-      </c>
-      <c r="O96" t="inlineStr">
+      <c r="R96" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="S96" t="inlineStr">
         <is>
           <t>27/09/2023 03:12</t>
         </is>
       </c>
-      <c r="P96" t="n">
-        <v>2.91</v>
-      </c>
-      <c r="Q96" t="inlineStr">
+      <c r="T96" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="U96" t="inlineStr">
         <is>
           <t>28/09/2023 15:59</t>
         </is>
       </c>
-      <c r="R96" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>27/09/2023 03:12</t>
-        </is>
-      </c>
-      <c r="T96" t="n">
-        <v>4.27</v>
-      </c>
-      <c r="U96" t="inlineStr">
-        <is>
-          <t>28/09/2023 15:59</t>
-        </is>
-      </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-svoge/CrS69OjU/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-spartak-varna/0KrZGlht/</t>
         </is>
       </c>
     </row>
@@ -9313,22 +9313,22 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Ludogorets II</t>
         </is>
       </c>
       <c r="G97" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Spartak Varna</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="I97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>2.15</v>
+        <v>1.88</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
@@ -9336,15 +9336,15 @@
         </is>
       </c>
       <c r="L97" t="n">
-        <v>1.93</v>
+        <v>1.89</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>28/09/2023 15:56</t>
+          <t>28/09/2023 15:59</t>
         </is>
       </c>
       <c r="N97" t="n">
-        <v>2.77</v>
+        <v>3.05</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -9352,7 +9352,7 @@
         </is>
       </c>
       <c r="P97" t="n">
-        <v>3.23</v>
+        <v>2.91</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
@@ -9360,7 +9360,7 @@
         </is>
       </c>
       <c r="R97" t="n">
-        <v>3.11</v>
+        <v>3.45</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
@@ -9368,7 +9368,7 @@
         </is>
       </c>
       <c r="T97" t="n">
-        <v>3.57</v>
+        <v>4.27</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-spartak-varna/0KrZGlht/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-svoge/CrS69OjU/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,14 +9781,14 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Septemvri Sofia</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J102" t="n">
-        <v>1.76</v>
+        <v>2.49</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
@@ -9796,15 +9796,15 @@
         </is>
       </c>
       <c r="L102" t="n">
-        <v>1.88</v>
+        <v>3.42</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>02/10/2023 14:57</t>
+          <t>02/10/2023 14:46</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.15</v>
+        <v>2.82</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
@@ -9812,15 +9812,15 @@
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.33</v>
+        <v>3.04</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>02/10/2023 14:57</t>
+          <t>02/10/2023 14:46</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>3.82</v>
+        <v>2.56</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
@@ -9828,16 +9828,16 @@
         </is>
       </c>
       <c r="T102" t="n">
-        <v>3.65</v>
+        <v>2.07</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>02/10/2023 14:57</t>
+          <t>02/10/2023 14:08</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-spartak-pleven/IqeTQPL4/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-septemvri-sofia/Ozybt5Li/</t>
         </is>
       </c>
     </row>
@@ -9957,7 +9957,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="G104" t="n">
@@ -9965,14 +9965,14 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Septemvri Sofia</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="I104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J104" t="n">
-        <v>2.49</v>
+        <v>1.76</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
@@ -9980,15 +9980,15 @@
         </is>
       </c>
       <c r="L104" t="n">
-        <v>3.42</v>
+        <v>1.88</v>
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>02/10/2023 14:46</t>
+          <t>02/10/2023 14:57</t>
         </is>
       </c>
       <c r="N104" t="n">
-        <v>2.82</v>
+        <v>3.15</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
@@ -9996,15 +9996,15 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>3.04</v>
+        <v>3.33</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>02/10/2023 14:46</t>
+          <t>02/10/2023 14:57</t>
         </is>
       </c>
       <c r="R104" t="n">
-        <v>2.56</v>
+        <v>3.82</v>
       </c>
       <c r="S104" t="inlineStr">
         <is>
@@ -10012,16 +10012,16 @@
         </is>
       </c>
       <c r="T104" t="n">
-        <v>2.07</v>
+        <v>3.65</v>
       </c>
       <c r="U104" t="inlineStr">
         <is>
-          <t>02/10/2023 14:08</t>
+          <t>02/10/2023 14:57</t>
         </is>
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-septemvri-sofia/Ozybt5Li/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-spartak-pleven/IqeTQPL4/</t>
         </is>
       </c>
     </row>
@@ -11245,22 +11245,22 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="G118" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>Ludogorets II</t>
+        </is>
+      </c>
+      <c r="I118" t="n">
         <v>2</v>
       </c>
-      <c r="H118" t="inlineStr">
-        <is>
-          <t>Svoge</t>
-        </is>
-      </c>
-      <c r="I118" t="n">
-        <v>0</v>
-      </c>
       <c r="J118" t="n">
-        <v>1.89</v>
+        <v>2.75</v>
       </c>
       <c r="K118" t="inlineStr">
         <is>
@@ -11268,15 +11268,15 @@
         </is>
       </c>
       <c r="L118" t="n">
-        <v>1.81</v>
+        <v>2.71</v>
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>21/10/2023 14:54</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="N118" t="n">
-        <v>2.94</v>
+        <v>2.81</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -11284,15 +11284,15 @@
         </is>
       </c>
       <c r="P118" t="n">
-        <v>3.18</v>
+        <v>2.85</v>
       </c>
       <c r="Q118" t="inlineStr">
         <is>
-          <t>21/10/2023 14:54</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="R118" t="n">
-        <v>3.71</v>
+        <v>2.34</v>
       </c>
       <c r="S118" t="inlineStr">
         <is>
@@ -11300,16 +11300,16 @@
         </is>
       </c>
       <c r="T118" t="n">
-        <v>4.22</v>
+        <v>2.6</v>
       </c>
       <c r="U118" t="inlineStr">
         <is>
-          <t>21/10/2023 14:54</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="V118" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-svoge/zeMXhr5c/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-ludogorets/OGEpjtkG/</t>
         </is>
       </c>
     </row>
@@ -11337,22 +11337,22 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="G119" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="I119" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J119" t="n">
-        <v>2.26</v>
+        <v>1.88</v>
       </c>
       <c r="K119" t="inlineStr">
         <is>
@@ -11360,15 +11360,15 @@
         </is>
       </c>
       <c r="L119" t="n">
-        <v>2.44</v>
+        <v>1.59</v>
       </c>
       <c r="M119" t="inlineStr">
         <is>
-          <t>21/10/2023 14:48</t>
+          <t>21/10/2023 14:51</t>
         </is>
       </c>
       <c r="N119" t="n">
-        <v>2.88</v>
+        <v>3.03</v>
       </c>
       <c r="O119" t="inlineStr">
         <is>
@@ -11376,15 +11376,15 @@
         </is>
       </c>
       <c r="P119" t="n">
-        <v>2.83</v>
+        <v>3.42</v>
       </c>
       <c r="Q119" t="inlineStr">
         <is>
-          <t>21/10/2023 14:48</t>
+          <t>21/10/2023 14:51</t>
         </is>
       </c>
       <c r="R119" t="n">
-        <v>2.8</v>
+        <v>3.48</v>
       </c>
       <c r="S119" t="inlineStr">
         <is>
@@ -11392,16 +11392,16 @@
         </is>
       </c>
       <c r="T119" t="n">
-        <v>2.93</v>
+        <v>5.4</v>
       </c>
       <c r="U119" t="inlineStr">
         <is>
-          <t>21/10/2023 14:48</t>
+          <t>21/10/2023 14:51</t>
         </is>
       </c>
       <c r="V119" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-montana/MifLqvSq/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-1919-spartak-pleven/UgFtiMZ9/</t>
         </is>
       </c>
     </row>
@@ -11429,22 +11429,22 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="G120" t="n">
+        <v>2</v>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Svoge</t>
+        </is>
+      </c>
+      <c r="I120" t="n">
         <v>0</v>
       </c>
-      <c r="H120" t="inlineStr">
-        <is>
-          <t>Ludogorets II</t>
-        </is>
-      </c>
-      <c r="I120" t="n">
-        <v>2</v>
-      </c>
       <c r="J120" t="n">
-        <v>2.75</v>
+        <v>1.89</v>
       </c>
       <c r="K120" t="inlineStr">
         <is>
@@ -11452,15 +11452,15 @@
         </is>
       </c>
       <c r="L120" t="n">
-        <v>2.71</v>
+        <v>1.81</v>
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 14:54</t>
         </is>
       </c>
       <c r="N120" t="n">
-        <v>2.81</v>
+        <v>2.94</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -11468,15 +11468,15 @@
         </is>
       </c>
       <c r="P120" t="n">
-        <v>2.85</v>
+        <v>3.18</v>
       </c>
       <c r="Q120" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 14:54</t>
         </is>
       </c>
       <c r="R120" t="n">
-        <v>2.34</v>
+        <v>3.71</v>
       </c>
       <c r="S120" t="inlineStr">
         <is>
@@ -11484,16 +11484,16 @@
         </is>
       </c>
       <c r="T120" t="n">
-        <v>2.6</v>
+        <v>4.22</v>
       </c>
       <c r="U120" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 14:54</t>
         </is>
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-ludogorets/OGEpjtkG/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-svoge/zeMXhr5c/</t>
         </is>
       </c>
     </row>
@@ -11521,22 +11521,22 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="G121" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="I121" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J121" t="n">
-        <v>1.88</v>
+        <v>2.26</v>
       </c>
       <c r="K121" t="inlineStr">
         <is>
@@ -11544,15 +11544,15 @@
         </is>
       </c>
       <c r="L121" t="n">
-        <v>1.59</v>
+        <v>2.44</v>
       </c>
       <c r="M121" t="inlineStr">
         <is>
-          <t>21/10/2023 14:51</t>
+          <t>21/10/2023 14:48</t>
         </is>
       </c>
       <c r="N121" t="n">
-        <v>3.03</v>
+        <v>2.88</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -11560,15 +11560,15 @@
         </is>
       </c>
       <c r="P121" t="n">
-        <v>3.42</v>
+        <v>2.83</v>
       </c>
       <c r="Q121" t="inlineStr">
         <is>
-          <t>21/10/2023 14:51</t>
+          <t>21/10/2023 14:48</t>
         </is>
       </c>
       <c r="R121" t="n">
-        <v>3.48</v>
+        <v>2.8</v>
       </c>
       <c r="S121" t="inlineStr">
         <is>
@@ -11576,16 +11576,16 @@
         </is>
       </c>
       <c r="T121" t="n">
-        <v>5.4</v>
+        <v>2.93</v>
       </c>
       <c r="U121" t="inlineStr">
         <is>
-          <t>21/10/2023 14:51</t>
+          <t>21/10/2023 14:48</t>
         </is>
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-1919-spartak-pleven/UgFtiMZ9/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-montana/MifLqvSq/</t>
         </is>
       </c>
     </row>
@@ -11613,71 +11613,71 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Yantra Gabrovo</t>
         </is>
       </c>
       <c r="G122" t="n">
+        <v>0</v>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>CSKA 1948 Sofia II</t>
+        </is>
+      </c>
+      <c r="I122" t="n">
         <v>1</v>
       </c>
-      <c r="H122" t="inlineStr">
-        <is>
-          <t>Strumska Slava</t>
-        </is>
-      </c>
-      <c r="I122" t="n">
-        <v>0</v>
-      </c>
       <c r="J122" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>21/10/2023 02:13</t>
+        </is>
+      </c>
+      <c r="L122" t="n">
         <v>1.81</v>
       </c>
-      <c r="K122" t="inlineStr">
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>22/10/2023 14:56</t>
+        </is>
+      </c>
+      <c r="N122" t="n">
+        <v>2.72</v>
+      </c>
+      <c r="O122" t="inlineStr">
         <is>
           <t>21/10/2023 02:13</t>
         </is>
       </c>
-      <c r="L122" t="n">
-        <v>1.62</v>
-      </c>
-      <c r="M122" t="inlineStr">
-        <is>
-          <t>22/10/2023 14:45</t>
-        </is>
-      </c>
-      <c r="N122" t="n">
-        <v>3.15</v>
-      </c>
-      <c r="O122" t="inlineStr">
+      <c r="P122" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>22/10/2023 14:58</t>
+        </is>
+      </c>
+      <c r="R122" t="n">
+        <v>3.03</v>
+      </c>
+      <c r="S122" t="inlineStr">
         <is>
           <t>21/10/2023 02:13</t>
         </is>
       </c>
-      <c r="P122" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="Q122" t="inlineStr">
-        <is>
-          <t>22/10/2023 14:45</t>
-        </is>
-      </c>
-      <c r="R122" t="n">
-        <v>3.74</v>
-      </c>
-      <c r="S122" t="inlineStr">
-        <is>
-          <t>21/10/2023 02:13</t>
-        </is>
-      </c>
       <c r="T122" t="n">
-        <v>5.05</v>
+        <v>4.56</v>
       </c>
       <c r="U122" t="inlineStr">
         <is>
-          <t>22/10/2023 14:45</t>
+          <t>22/10/2023 14:57</t>
         </is>
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-strumska-slava/GEgPrbsj/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/yantra-gabrovo-cska-1948-sofia/IJBxh2K3/</t>
         </is>
       </c>
     </row>
@@ -11705,22 +11705,22 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Yantra Gabrovo</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="G123" t="n">
+        <v>1</v>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Strumska Slava</t>
+        </is>
+      </c>
+      <c r="I123" t="n">
         <v>0</v>
       </c>
-      <c r="H123" t="inlineStr">
-        <is>
-          <t>CSKA 1948 Sofia II</t>
-        </is>
-      </c>
-      <c r="I123" t="n">
-        <v>1</v>
-      </c>
       <c r="J123" t="n">
-        <v>2.28</v>
+        <v>1.81</v>
       </c>
       <c r="K123" t="inlineStr">
         <is>
@@ -11728,15 +11728,15 @@
         </is>
       </c>
       <c r="L123" t="n">
-        <v>1.81</v>
+        <v>1.62</v>
       </c>
       <c r="M123" t="inlineStr">
         <is>
-          <t>22/10/2023 14:56</t>
+          <t>22/10/2023 14:45</t>
         </is>
       </c>
       <c r="N123" t="n">
-        <v>2.72</v>
+        <v>3.15</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -11744,15 +11744,15 @@
         </is>
       </c>
       <c r="P123" t="n">
-        <v>3.01</v>
+        <v>3.45</v>
       </c>
       <c r="Q123" t="inlineStr">
         <is>
-          <t>22/10/2023 14:58</t>
+          <t>22/10/2023 14:45</t>
         </is>
       </c>
       <c r="R123" t="n">
-        <v>3.03</v>
+        <v>3.74</v>
       </c>
       <c r="S123" t="inlineStr">
         <is>
@@ -11760,16 +11760,16 @@
         </is>
       </c>
       <c r="T123" t="n">
-        <v>4.56</v>
+        <v>5.05</v>
       </c>
       <c r="U123" t="inlineStr">
         <is>
-          <t>22/10/2023 14:57</t>
+          <t>22/10/2023 14:45</t>
         </is>
       </c>
       <c r="V123" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/yantra-gabrovo-cska-1948-sofia/IJBxh2K3/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-strumska-slava/GEgPrbsj/</t>
         </is>
       </c>
     </row>
@@ -12717,22 +12717,22 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="G134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Yantra Gabrovo</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="I134" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J134" t="n">
-        <v>2.15</v>
+        <v>1.36</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -12740,15 +12740,15 @@
         </is>
       </c>
       <c r="L134" t="n">
-        <v>2.42</v>
+        <v>1.37</v>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>03/11/2023 12:25</t>
+          <t>03/11/2023 12:42</t>
         </is>
       </c>
       <c r="N134" t="n">
-        <v>2.79</v>
+        <v>3.94</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -12756,15 +12756,15 @@
         </is>
       </c>
       <c r="P134" t="n">
-        <v>2.78</v>
+        <v>4.03</v>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>03/11/2023 12:25</t>
+          <t>03/11/2023 13:18</t>
         </is>
       </c>
       <c r="R134" t="n">
-        <v>3.09</v>
+        <v>6.19</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -12772,16 +12772,16 @@
         </is>
       </c>
       <c r="T134" t="n">
-        <v>3.01</v>
+        <v>8.08</v>
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>03/11/2023 12:25</t>
+          <t>03/11/2023 13:18</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-yantra-gabrovo/6LcCs92D/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-strumska-slava/KONod8H6/</t>
         </is>
       </c>
     </row>
@@ -12809,22 +12809,22 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="G135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="I135" t="n">
         <v>2</v>
       </c>
       <c r="J135" t="n">
-        <v>1.36</v>
+        <v>1.91</v>
       </c>
       <c r="K135" t="inlineStr">
         <is>
@@ -12832,15 +12832,15 @@
         </is>
       </c>
       <c r="L135" t="n">
-        <v>1.37</v>
+        <v>1.72</v>
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>03/11/2023 12:42</t>
+          <t>03/11/2023 13:26</t>
         </is>
       </c>
       <c r="N135" t="n">
-        <v>3.94</v>
+        <v>2.97</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -12848,15 +12848,15 @@
         </is>
       </c>
       <c r="P135" t="n">
-        <v>4.03</v>
+        <v>3.23</v>
       </c>
       <c r="Q135" t="inlineStr">
         <is>
-          <t>03/11/2023 13:18</t>
+          <t>03/11/2023 13:26</t>
         </is>
       </c>
       <c r="R135" t="n">
-        <v>6.19</v>
+        <v>3.48</v>
       </c>
       <c r="S135" t="inlineStr">
         <is>
@@ -12864,16 +12864,16 @@
         </is>
       </c>
       <c r="T135" t="n">
-        <v>8.08</v>
+        <v>4.67</v>
       </c>
       <c r="U135" t="inlineStr">
         <is>
-          <t>03/11/2023 13:18</t>
+          <t>03/11/2023 12:47</t>
         </is>
       </c>
       <c r="V135" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-strumska-slava/KONod8H6/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-1919-svoge/KOof6huE/</t>
         </is>
       </c>
     </row>
@@ -12901,22 +12901,22 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Belasitsa</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="G136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Yantra Gabrovo</t>
         </is>
       </c>
       <c r="I136" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J136" t="n">
-        <v>1.94</v>
+        <v>2.15</v>
       </c>
       <c r="K136" t="inlineStr">
         <is>
@@ -12924,15 +12924,15 @@
         </is>
       </c>
       <c r="L136" t="n">
-        <v>1.64</v>
+        <v>2.42</v>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>03/11/2023 13:29</t>
+          <t>03/11/2023 12:25</t>
         </is>
       </c>
       <c r="N136" t="n">
-        <v>2.98</v>
+        <v>2.79</v>
       </c>
       <c r="O136" t="inlineStr">
         <is>
@@ -12940,15 +12940,15 @@
         </is>
       </c>
       <c r="P136" t="n">
-        <v>3.49</v>
+        <v>2.78</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
-          <t>03/11/2023 13:29</t>
+          <t>03/11/2023 12:25</t>
         </is>
       </c>
       <c r="R136" t="n">
-        <v>3.35</v>
+        <v>3.09</v>
       </c>
       <c r="S136" t="inlineStr">
         <is>
@@ -12956,16 +12956,16 @@
         </is>
       </c>
       <c r="T136" t="n">
-        <v>4.74</v>
+        <v>3.01</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>03/11/2023 13:29</t>
+          <t>03/11/2023 12:25</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/belasitsa-petrich-spartak-pleven/ENv34W9Q/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-yantra-gabrovo/6LcCs92D/</t>
         </is>
       </c>
     </row>
@@ -13085,22 +13085,22 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Belasitsa</t>
         </is>
       </c>
       <c r="G138" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="I138" t="n">
         <v>2</v>
       </c>
       <c r="J138" t="n">
-        <v>1.91</v>
+        <v>1.94</v>
       </c>
       <c r="K138" t="inlineStr">
         <is>
@@ -13108,15 +13108,15 @@
         </is>
       </c>
       <c r="L138" t="n">
-        <v>1.72</v>
+        <v>1.64</v>
       </c>
       <c r="M138" t="inlineStr">
         <is>
-          <t>03/11/2023 13:26</t>
+          <t>03/11/2023 13:29</t>
         </is>
       </c>
       <c r="N138" t="n">
-        <v>2.97</v>
+        <v>2.98</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -13124,15 +13124,15 @@
         </is>
       </c>
       <c r="P138" t="n">
-        <v>3.23</v>
+        <v>3.49</v>
       </c>
       <c r="Q138" t="inlineStr">
         <is>
-          <t>03/11/2023 13:26</t>
+          <t>03/11/2023 13:29</t>
         </is>
       </c>
       <c r="R138" t="n">
-        <v>3.48</v>
+        <v>3.35</v>
       </c>
       <c r="S138" t="inlineStr">
         <is>
@@ -13140,16 +13140,16 @@
         </is>
       </c>
       <c r="T138" t="n">
-        <v>4.67</v>
+        <v>4.74</v>
       </c>
       <c r="U138" t="inlineStr">
         <is>
-          <t>03/11/2023 12:47</t>
+          <t>03/11/2023 13:29</t>
         </is>
       </c>
       <c r="V138" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-1919-svoge/KOof6huE/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/belasitsa-petrich-spartak-pleven/ENv34W9Q/</t>
         </is>
       </c>
     </row>
@@ -13821,22 +13821,22 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="G146" t="n">
+        <v>0</v>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Septemvri Sofia</t>
+        </is>
+      </c>
+      <c r="I146" t="n">
         <v>2</v>
       </c>
-      <c r="H146" t="inlineStr">
-        <is>
-          <t>Bdin Vidin</t>
-        </is>
-      </c>
-      <c r="I146" t="n">
-        <v>0</v>
-      </c>
       <c r="J146" t="n">
-        <v>1.64</v>
+        <v>5.09</v>
       </c>
       <c r="K146" t="inlineStr">
         <is>
@@ -13844,48 +13844,48 @@
         </is>
       </c>
       <c r="L146" t="n">
+        <v>6.24</v>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>12/11/2023 13:15</t>
+        </is>
+      </c>
+      <c r="N146" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="O146" t="inlineStr">
+        <is>
+          <t>12/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="P146" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="Q146" t="inlineStr">
+        <is>
+          <t>12/11/2023 13:15</t>
+        </is>
+      </c>
+      <c r="R146" t="n">
         <v>1.56</v>
       </c>
-      <c r="M146" t="inlineStr">
-        <is>
-          <t>12/11/2023 13:28</t>
-        </is>
-      </c>
-      <c r="N146" t="n">
-        <v>3.34</v>
-      </c>
-      <c r="O146" t="inlineStr">
+      <c r="S146" t="inlineStr">
         <is>
           <t>12/11/2023 02:42</t>
         </is>
       </c>
-      <c r="P146" t="n">
-        <v>3.44</v>
-      </c>
-      <c r="Q146" t="inlineStr">
-        <is>
-          <t>12/11/2023 13:28</t>
-        </is>
-      </c>
-      <c r="R146" t="n">
-        <v>4.93</v>
-      </c>
-      <c r="S146" t="inlineStr">
-        <is>
-          <t>12/11/2023 02:42</t>
-        </is>
-      </c>
       <c r="T146" t="n">
-        <v>5.77</v>
+        <v>1.46</v>
       </c>
       <c r="U146" t="inlineStr">
         <is>
-          <t>12/11/2023 13:28</t>
+          <t>12/11/2023 13:15</t>
         </is>
       </c>
       <c r="V146" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-bdin-vidin/OI5DA7Wa/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-septemvri-sofia/hURUIVOJ/</t>
         </is>
       </c>
     </row>
@@ -13913,22 +13913,22 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>Litex Lovech</t>
         </is>
       </c>
       <c r="G147" t="n">
+        <v>1</v>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Dunav Ruse</t>
+        </is>
+      </c>
+      <c r="I147" t="n">
         <v>0</v>
       </c>
-      <c r="H147" t="inlineStr">
-        <is>
-          <t>Septemvri Sofia</t>
-        </is>
-      </c>
-      <c r="I147" t="n">
-        <v>2</v>
-      </c>
       <c r="J147" t="n">
-        <v>5.09</v>
+        <v>2.62</v>
       </c>
       <c r="K147" t="inlineStr">
         <is>
@@ -13936,48 +13936,48 @@
         </is>
       </c>
       <c r="L147" t="n">
-        <v>6.24</v>
+        <v>2.06</v>
       </c>
       <c r="M147" t="inlineStr">
         <is>
-          <t>12/11/2023 13:15</t>
+          <t>12/11/2023 13:22</t>
         </is>
       </c>
       <c r="N147" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>12/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="P147" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>12/11/2023 13:22</t>
+        </is>
+      </c>
+      <c r="R147" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="S147" t="inlineStr">
+        <is>
+          <t>12/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="T147" t="n">
         <v>3.54</v>
       </c>
-      <c r="O147" t="inlineStr">
-        <is>
-          <t>12/11/2023 02:42</t>
-        </is>
-      </c>
-      <c r="P147" t="n">
-        <v>3.84</v>
-      </c>
-      <c r="Q147" t="inlineStr">
-        <is>
-          <t>12/11/2023 13:15</t>
-        </is>
-      </c>
-      <c r="R147" t="n">
-        <v>1.56</v>
-      </c>
-      <c r="S147" t="inlineStr">
-        <is>
-          <t>12/11/2023 02:42</t>
-        </is>
-      </c>
-      <c r="T147" t="n">
-        <v>1.46</v>
-      </c>
       <c r="U147" t="inlineStr">
         <is>
-          <t>12/11/2023 13:15</t>
+          <t>12/11/2023 13:22</t>
         </is>
       </c>
       <c r="V147" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-septemvri-sofia/hURUIVOJ/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/litex-lovech-dunav-ruse/WKQYHkvQ/</t>
         </is>
       </c>
     </row>
@@ -14005,22 +14005,22 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>Litex Lovech</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="G148" t="n">
+        <v>2</v>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Spartak Varna</t>
+        </is>
+      </c>
+      <c r="I148" t="n">
         <v>1</v>
       </c>
-      <c r="H148" t="inlineStr">
-        <is>
-          <t>Dunav Ruse</t>
-        </is>
-      </c>
-      <c r="I148" t="n">
-        <v>0</v>
-      </c>
       <c r="J148" t="n">
-        <v>2.62</v>
+        <v>4.82</v>
       </c>
       <c r="K148" t="inlineStr">
         <is>
@@ -14028,15 +14028,15 @@
         </is>
       </c>
       <c r="L148" t="n">
-        <v>2.06</v>
+        <v>5.52</v>
       </c>
       <c r="M148" t="inlineStr">
         <is>
-          <t>12/11/2023 13:22</t>
+          <t>12/11/2023 12:36</t>
         </is>
       </c>
       <c r="N148" t="n">
-        <v>2.74</v>
+        <v>3.49</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -14044,15 +14044,15 @@
         </is>
       </c>
       <c r="P148" t="n">
-        <v>2.96</v>
+        <v>3.67</v>
       </c>
       <c r="Q148" t="inlineStr">
         <is>
-          <t>12/11/2023 13:22</t>
+          <t>12/11/2023 12:36</t>
         </is>
       </c>
       <c r="R148" t="n">
-        <v>2.75</v>
+        <v>1.59</v>
       </c>
       <c r="S148" t="inlineStr">
         <is>
@@ -14060,16 +14060,16 @@
         </is>
       </c>
       <c r="T148" t="n">
-        <v>3.54</v>
+        <v>1.53</v>
       </c>
       <c r="U148" t="inlineStr">
         <is>
-          <t>12/11/2023 13:22</t>
+          <t>12/11/2023 12:36</t>
         </is>
       </c>
       <c r="V148" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/litex-lovech-dunav-ruse/WKQYHkvQ/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-spartak-varna/23H4CT1m/</t>
         </is>
       </c>
     </row>
@@ -14097,22 +14097,22 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="G149" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>Spartak Varna</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="I149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J149" t="n">
-        <v>4.82</v>
+        <v>2.09</v>
       </c>
       <c r="K149" t="inlineStr">
         <is>
@@ -14120,15 +14120,15 @@
         </is>
       </c>
       <c r="L149" t="n">
-        <v>5.52</v>
+        <v>1.8</v>
       </c>
       <c r="M149" t="inlineStr">
         <is>
-          <t>12/11/2023 12:36</t>
+          <t>12/11/2023 13:06</t>
         </is>
       </c>
       <c r="N149" t="n">
-        <v>3.49</v>
+        <v>2.93</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -14136,15 +14136,15 @@
         </is>
       </c>
       <c r="P149" t="n">
-        <v>3.67</v>
+        <v>3.09</v>
       </c>
       <c r="Q149" t="inlineStr">
         <is>
-          <t>12/11/2023 12:36</t>
+          <t>12/11/2023 13:06</t>
         </is>
       </c>
       <c r="R149" t="n">
-        <v>1.59</v>
+        <v>3.33</v>
       </c>
       <c r="S149" t="inlineStr">
         <is>
@@ -14152,16 +14152,16 @@
         </is>
       </c>
       <c r="T149" t="n">
-        <v>1.53</v>
+        <v>4.41</v>
       </c>
       <c r="U149" t="inlineStr">
         <is>
-          <t>12/11/2023 12:36</t>
+          <t>12/11/2023 13:06</t>
         </is>
       </c>
       <c r="V149" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-spartak-varna/23H4CT1m/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-marek/EoNkeSWC/</t>
         </is>
       </c>
     </row>
@@ -14189,22 +14189,22 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="G150" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="I150" t="n">
         <v>0</v>
       </c>
       <c r="J150" t="n">
-        <v>2.09</v>
+        <v>1.64</v>
       </c>
       <c r="K150" t="inlineStr">
         <is>
@@ -14212,15 +14212,15 @@
         </is>
       </c>
       <c r="L150" t="n">
-        <v>1.8</v>
+        <v>1.56</v>
       </c>
       <c r="M150" t="inlineStr">
         <is>
-          <t>12/11/2023 13:06</t>
+          <t>12/11/2023 13:28</t>
         </is>
       </c>
       <c r="N150" t="n">
-        <v>2.93</v>
+        <v>3.34</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -14228,15 +14228,15 @@
         </is>
       </c>
       <c r="P150" t="n">
-        <v>3.09</v>
+        <v>3.44</v>
       </c>
       <c r="Q150" t="inlineStr">
         <is>
-          <t>12/11/2023 13:06</t>
+          <t>12/11/2023 13:28</t>
         </is>
       </c>
       <c r="R150" t="n">
-        <v>3.33</v>
+        <v>4.93</v>
       </c>
       <c r="S150" t="inlineStr">
         <is>
@@ -14244,16 +14244,16 @@
         </is>
       </c>
       <c r="T150" t="n">
-        <v>4.41</v>
+        <v>5.77</v>
       </c>
       <c r="U150" t="inlineStr">
         <is>
-          <t>12/11/2023 13:06</t>
+          <t>12/11/2023 13:28</t>
         </is>
       </c>
       <c r="V150" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-marek/EoNkeSWC/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-bdin-vidin/OI5DA7Wa/</t>
         </is>
       </c>
     </row>
@@ -14346,6 +14346,98 @@
       <c r="V151" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-dobrudzha/hxMgfnnJ/</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>bulgaria</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>vtora-liga</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E152" s="2" t="n">
+        <v>45247.5625</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Yantra Gabrovo</t>
+        </is>
+      </c>
+      <c r="G152" t="n">
+        <v>1</v>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>Ludogorets II</t>
+        </is>
+      </c>
+      <c r="I152" t="n">
+        <v>1</v>
+      </c>
+      <c r="J152" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>17/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="L152" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>17/11/2023 13:28</t>
+        </is>
+      </c>
+      <c r="N152" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="O152" t="inlineStr">
+        <is>
+          <t>17/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="P152" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="Q152" t="inlineStr">
+        <is>
+          <t>17/11/2023 13:28</t>
+        </is>
+      </c>
+      <c r="R152" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="S152" t="inlineStr">
+        <is>
+          <t>17/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="T152" t="n">
+        <v>5.19</v>
+      </c>
+      <c r="U152" t="inlineStr">
+        <is>
+          <t>17/11/2023 13:28</t>
+        </is>
+      </c>
+      <c r="V152" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/yantra-gabrovo-ludogorets/GUDWPqyB/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 23-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/bulgaria_vtora-liga_2023-2024.xlsx
+++ b/2023/bulgaria_vtora-liga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V152"/>
+  <dimension ref="A1:V153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12717,22 +12717,22 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="G134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>CSKA 1948 Sofia II</t>
         </is>
       </c>
       <c r="I134" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J134" t="n">
-        <v>1.36</v>
+        <v>4.31</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -12740,15 +12740,15 @@
         </is>
       </c>
       <c r="L134" t="n">
-        <v>1.37</v>
+        <v>4.54</v>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>03/11/2023 12:42</t>
+          <t>03/11/2023 13:23</t>
         </is>
       </c>
       <c r="N134" t="n">
-        <v>3.94</v>
+        <v>3.15</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -12756,15 +12756,15 @@
         </is>
       </c>
       <c r="P134" t="n">
-        <v>4.03</v>
+        <v>2.8</v>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>03/11/2023 13:18</t>
+          <t>03/11/2023 13:23</t>
         </is>
       </c>
       <c r="R134" t="n">
-        <v>6.19</v>
+        <v>1.67</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -12772,16 +12772,16 @@
         </is>
       </c>
       <c r="T134" t="n">
-        <v>8.08</v>
+        <v>1.89</v>
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>03/11/2023 13:18</t>
+          <t>03/11/2023 13:23</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-strumska-slava/KONod8H6/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-cska-1948-sofia/Wbkb5CfK/</t>
         </is>
       </c>
     </row>
@@ -12809,22 +12809,22 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Belasitsa</t>
         </is>
       </c>
       <c r="G135" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="I135" t="n">
         <v>2</v>
       </c>
       <c r="J135" t="n">
-        <v>1.91</v>
+        <v>1.94</v>
       </c>
       <c r="K135" t="inlineStr">
         <is>
@@ -12832,15 +12832,15 @@
         </is>
       </c>
       <c r="L135" t="n">
-        <v>1.72</v>
+        <v>1.64</v>
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>03/11/2023 13:26</t>
+          <t>03/11/2023 13:29</t>
         </is>
       </c>
       <c r="N135" t="n">
-        <v>2.97</v>
+        <v>2.98</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -12848,15 +12848,15 @@
         </is>
       </c>
       <c r="P135" t="n">
-        <v>3.23</v>
+        <v>3.49</v>
       </c>
       <c r="Q135" t="inlineStr">
         <is>
-          <t>03/11/2023 13:26</t>
+          <t>03/11/2023 13:29</t>
         </is>
       </c>
       <c r="R135" t="n">
-        <v>3.48</v>
+        <v>3.35</v>
       </c>
       <c r="S135" t="inlineStr">
         <is>
@@ -12864,16 +12864,16 @@
         </is>
       </c>
       <c r="T135" t="n">
-        <v>4.67</v>
+        <v>4.74</v>
       </c>
       <c r="U135" t="inlineStr">
         <is>
-          <t>03/11/2023 12:47</t>
+          <t>03/11/2023 13:29</t>
         </is>
       </c>
       <c r="V135" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-1919-svoge/KOof6huE/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/belasitsa-petrich-spartak-pleven/ENv34W9Q/</t>
         </is>
       </c>
     </row>
@@ -12901,7 +12901,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -12909,14 +12909,14 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Yantra Gabrovo</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="I136" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J136" t="n">
-        <v>2.15</v>
+        <v>1.91</v>
       </c>
       <c r="K136" t="inlineStr">
         <is>
@@ -12924,15 +12924,15 @@
         </is>
       </c>
       <c r="L136" t="n">
-        <v>2.42</v>
+        <v>1.72</v>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>03/11/2023 12:25</t>
+          <t>03/11/2023 13:26</t>
         </is>
       </c>
       <c r="N136" t="n">
-        <v>2.79</v>
+        <v>2.97</v>
       </c>
       <c r="O136" t="inlineStr">
         <is>
@@ -12940,15 +12940,15 @@
         </is>
       </c>
       <c r="P136" t="n">
-        <v>2.78</v>
+        <v>3.23</v>
       </c>
       <c r="Q136" t="inlineStr">
         <is>
-          <t>03/11/2023 12:25</t>
+          <t>03/11/2023 13:26</t>
         </is>
       </c>
       <c r="R136" t="n">
-        <v>3.09</v>
+        <v>3.48</v>
       </c>
       <c r="S136" t="inlineStr">
         <is>
@@ -12956,16 +12956,16 @@
         </is>
       </c>
       <c r="T136" t="n">
-        <v>3.01</v>
+        <v>4.67</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>03/11/2023 12:25</t>
+          <t>03/11/2023 12:47</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-yantra-gabrovo/6LcCs92D/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-1919-svoge/KOof6huE/</t>
         </is>
       </c>
     </row>
@@ -12993,22 +12993,22 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="G137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>CSKA 1948 Sofia II</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="I137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J137" t="n">
-        <v>4.31</v>
+        <v>1.36</v>
       </c>
       <c r="K137" t="inlineStr">
         <is>
@@ -13016,15 +13016,15 @@
         </is>
       </c>
       <c r="L137" t="n">
-        <v>4.54</v>
+        <v>1.37</v>
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>03/11/2023 13:23</t>
+          <t>03/11/2023 12:42</t>
         </is>
       </c>
       <c r="N137" t="n">
-        <v>3.15</v>
+        <v>3.94</v>
       </c>
       <c r="O137" t="inlineStr">
         <is>
@@ -13032,15 +13032,15 @@
         </is>
       </c>
       <c r="P137" t="n">
-        <v>2.8</v>
+        <v>4.03</v>
       </c>
       <c r="Q137" t="inlineStr">
         <is>
-          <t>03/11/2023 13:23</t>
+          <t>03/11/2023 13:18</t>
         </is>
       </c>
       <c r="R137" t="n">
-        <v>1.67</v>
+        <v>6.19</v>
       </c>
       <c r="S137" t="inlineStr">
         <is>
@@ -13048,16 +13048,16 @@
         </is>
       </c>
       <c r="T137" t="n">
-        <v>1.89</v>
+        <v>8.08</v>
       </c>
       <c r="U137" t="inlineStr">
         <is>
-          <t>03/11/2023 13:23</t>
+          <t>03/11/2023 13:18</t>
         </is>
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-cska-1948-sofia/Wbkb5CfK/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-strumska-slava/KONod8H6/</t>
         </is>
       </c>
     </row>
@@ -13085,22 +13085,22 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Belasitsa</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="G138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Yantra Gabrovo</t>
         </is>
       </c>
       <c r="I138" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J138" t="n">
-        <v>1.94</v>
+        <v>2.15</v>
       </c>
       <c r="K138" t="inlineStr">
         <is>
@@ -13108,15 +13108,15 @@
         </is>
       </c>
       <c r="L138" t="n">
-        <v>1.64</v>
+        <v>2.42</v>
       </c>
       <c r="M138" t="inlineStr">
         <is>
-          <t>03/11/2023 13:29</t>
+          <t>03/11/2023 12:25</t>
         </is>
       </c>
       <c r="N138" t="n">
-        <v>2.98</v>
+        <v>2.79</v>
       </c>
       <c r="O138" t="inlineStr">
         <is>
@@ -13124,15 +13124,15 @@
         </is>
       </c>
       <c r="P138" t="n">
-        <v>3.49</v>
+        <v>2.78</v>
       </c>
       <c r="Q138" t="inlineStr">
         <is>
-          <t>03/11/2023 13:29</t>
+          <t>03/11/2023 12:25</t>
         </is>
       </c>
       <c r="R138" t="n">
-        <v>3.35</v>
+        <v>3.09</v>
       </c>
       <c r="S138" t="inlineStr">
         <is>
@@ -13140,16 +13140,16 @@
         </is>
       </c>
       <c r="T138" t="n">
-        <v>4.74</v>
+        <v>3.01</v>
       </c>
       <c r="U138" t="inlineStr">
         <is>
-          <t>03/11/2023 13:29</t>
+          <t>03/11/2023 12:25</t>
         </is>
       </c>
       <c r="V138" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/belasitsa-petrich-spartak-pleven/ENv34W9Q/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-yantra-gabrovo/6LcCs92D/</t>
         </is>
       </c>
     </row>
@@ -14438,6 +14438,98 @@
       <c r="V152" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/yantra-gabrovo-ludogorets/GUDWPqyB/</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>bulgaria</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>vtora-liga</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E153" s="2" t="n">
+        <v>45253.5625</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Ludogorets II</t>
+        </is>
+      </c>
+      <c r="G153" t="n">
+        <v>0</v>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>Chernomorets 1919</t>
+        </is>
+      </c>
+      <c r="I153" t="n">
+        <v>1</v>
+      </c>
+      <c r="J153" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>22/11/2023 15:14</t>
+        </is>
+      </c>
+      <c r="L153" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>23/11/2023 12:03</t>
+        </is>
+      </c>
+      <c r="N153" t="n">
+        <v>3.41</v>
+      </c>
+      <c r="O153" t="inlineStr">
+        <is>
+          <t>22/11/2023 15:14</t>
+        </is>
+      </c>
+      <c r="P153" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>23/11/2023 12:56</t>
+        </is>
+      </c>
+      <c r="R153" t="n">
+        <v>5</v>
+      </c>
+      <c r="S153" t="inlineStr">
+        <is>
+          <t>22/11/2023 15:14</t>
+        </is>
+      </c>
+      <c r="T153" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="U153" t="inlineStr">
+        <is>
+          <t>23/11/2023 12:56</t>
+        </is>
+      </c>
+      <c r="V153" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-chernomorets-1919/UcVsWKcp/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 27-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/bulgaria_vtora-liga_2023-2024.xlsx
+++ b/2023/bulgaria_vtora-liga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V157"/>
+  <dimension ref="A1:V158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1677,71 +1677,71 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Litex Lovech</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>2.42</v>
+        <v>3.9</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>21/07/2023 06:42</t>
+          <t>22/07/2023 16:45</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>3.82</v>
+        <v>2.88</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>22/07/2023 18:29</t>
+          <t>22/07/2023 18:18</t>
         </is>
       </c>
       <c r="N14" t="n">
-        <v>2.69</v>
+        <v>3.59</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>21/07/2023 06:42</t>
+          <t>22/07/2023 16:45</t>
         </is>
       </c>
       <c r="P14" t="n">
-        <v>3</v>
+        <v>3.48</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>22/07/2023 18:24</t>
+          <t>22/07/2023 18:18</t>
         </is>
       </c>
       <c r="R14" t="n">
-        <v>2.78</v>
+        <v>1.75</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>21/07/2023 06:42</t>
+          <t>22/07/2023 16:45</t>
         </is>
       </c>
       <c r="T14" t="n">
-        <v>1.79</v>
+        <v>2.13</v>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>22/07/2023 18:29</t>
+          <t>22/07/2023 18:18</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/litex-lovech-dobrudzha/pC6LRjl8/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-strumska-slava/r7Sx37B7/</t>
         </is>
       </c>
     </row>
@@ -1769,71 +1769,71 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>Litex Lovech</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>3.9</v>
+        <v>2.42</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>22/07/2023 16:45</t>
+          <t>21/07/2023 06:42</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>2.88</v>
+        <v>3.82</v>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>22/07/2023 18:18</t>
+          <t>22/07/2023 18:29</t>
         </is>
       </c>
       <c r="N15" t="n">
-        <v>3.59</v>
+        <v>2.69</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>22/07/2023 16:45</t>
+          <t>21/07/2023 06:42</t>
         </is>
       </c>
       <c r="P15" t="n">
-        <v>3.48</v>
+        <v>3</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>22/07/2023 18:18</t>
+          <t>22/07/2023 18:24</t>
         </is>
       </c>
       <c r="R15" t="n">
-        <v>1.75</v>
+        <v>2.78</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>22/07/2023 16:45</t>
+          <t>21/07/2023 06:42</t>
         </is>
       </c>
       <c r="T15" t="n">
-        <v>2.13</v>
+        <v>1.79</v>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>22/07/2023 18:18</t>
+          <t>22/07/2023 18:29</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-strumska-slava/r7Sx37B7/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/litex-lovech-dobrudzha/pC6LRjl8/</t>
         </is>
       </c>
     </row>
@@ -2229,71 +2229,71 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Litex Lovech</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J20" t="n">
-        <v>2.85</v>
+        <v>2.08</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>29/07/2023 13:12</t>
+          <t>28/07/2023 05:42</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>2.73</v>
+        <v>2.01</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>29/07/2023 16:46</t>
+          <t>29/07/2023 17:02</t>
         </is>
       </c>
       <c r="N20" t="n">
-        <v>2.97</v>
+        <v>2.82</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>29/07/2023 13:12</t>
+          <t>28/07/2023 05:42</t>
         </is>
       </c>
       <c r="P20" t="n">
-        <v>3.27</v>
+        <v>2.9</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>29/07/2023 16:46</t>
+          <t>29/07/2023 17:02</t>
         </is>
       </c>
       <c r="R20" t="n">
-        <v>2.36</v>
+        <v>3.21</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>29/07/2023 13:12</t>
+          <t>28/07/2023 05:42</t>
         </is>
       </c>
       <c r="T20" t="n">
-        <v>2.31</v>
+        <v>3.78</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>29/07/2023 16:46</t>
+          <t>29/07/2023 17:02</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-marek/McmCH6Q0/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-litex-lovech/OvPtXoQm/</t>
         </is>
       </c>
     </row>
@@ -2321,22 +2321,22 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>CSKA 1948 Sofia II</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
         <v>2</v>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Litex Lovech</t>
-        </is>
-      </c>
-      <c r="I21" t="n">
-        <v>3</v>
-      </c>
       <c r="J21" t="n">
-        <v>2.08</v>
+        <v>2.62</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -2344,15 +2344,15 @@
         </is>
       </c>
       <c r="L21" t="n">
-        <v>2.01</v>
+        <v>2.39</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>29/07/2023 17:02</t>
+          <t>29/07/2023 16:28</t>
         </is>
       </c>
       <c r="N21" t="n">
-        <v>2.82</v>
+        <v>2.84</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2360,15 +2360,15 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>2.9</v>
+        <v>3.18</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>29/07/2023 17:02</t>
+          <t>29/07/2023 15:36</t>
         </is>
       </c>
       <c r="R21" t="n">
-        <v>3.21</v>
+        <v>2.48</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
@@ -2376,16 +2376,16 @@
         </is>
       </c>
       <c r="T21" t="n">
-        <v>3.78</v>
+        <v>2.69</v>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>29/07/2023 17:02</t>
+          <t>29/07/2023 16:28</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-litex-lovech/OvPtXoQm/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-cska-1948-sofia/pWY6wlmK/</t>
         </is>
       </c>
     </row>
@@ -2413,22 +2413,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="G22" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Ludogorets II</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
         <v>0</v>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>CSKA 1948 Sofia II</t>
-        </is>
-      </c>
-      <c r="I22" t="n">
-        <v>2</v>
-      </c>
       <c r="J22" t="n">
-        <v>2.62</v>
+        <v>1.5</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -2436,15 +2436,15 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>2.39</v>
+        <v>1.5</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>29/07/2023 16:28</t>
+          <t>29/07/2023 17:03</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>2.84</v>
+        <v>3.63</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2452,15 +2452,15 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.18</v>
+        <v>3.82</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>29/07/2023 15:36</t>
+          <t>29/07/2023 17:03</t>
         </is>
       </c>
       <c r="R22" t="n">
-        <v>2.48</v>
+        <v>5.07</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
@@ -2468,16 +2468,16 @@
         </is>
       </c>
       <c r="T22" t="n">
-        <v>2.69</v>
+        <v>5.69</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>29/07/2023 16:28</t>
+          <t>29/07/2023 17:03</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-cska-1948-sofia/pWY6wlmK/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-ludogorets/U3AwYRAs/</t>
         </is>
       </c>
     </row>
@@ -2505,71 +2505,71 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Marek</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
         <v>1</v>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Ludogorets II</t>
-        </is>
-      </c>
-      <c r="I23" t="n">
-        <v>0</v>
-      </c>
       <c r="J23" t="n">
-        <v>1.5</v>
+        <v>2.85</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>28/07/2023 05:42</t>
+          <t>29/07/2023 13:12</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>1.5</v>
+        <v>2.73</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>29/07/2023 17:03</t>
+          <t>29/07/2023 16:46</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>3.63</v>
+        <v>2.97</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>28/07/2023 05:42</t>
+          <t>29/07/2023 13:12</t>
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3.82</v>
+        <v>3.27</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>29/07/2023 17:03</t>
+          <t>29/07/2023 16:46</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>5.07</v>
+        <v>2.36</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>28/07/2023 05:42</t>
+          <t>29/07/2023 13:12</t>
         </is>
       </c>
       <c r="T23" t="n">
-        <v>5.69</v>
+        <v>2.31</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>29/07/2023 17:03</t>
+          <t>29/07/2023 16:46</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-ludogorets/U3AwYRAs/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-marek/McmCH6Q0/</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Belasitsa</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -2605,14 +2605,14 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>1.92</v>
+        <v>1.5</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -2620,15 +2620,15 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>1.93</v>
+        <v>1.42</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>29/07/2023 18:58</t>
+          <t>29/07/2023 18:03</t>
         </is>
       </c>
       <c r="N24" t="n">
-        <v>3.07</v>
+        <v>3.96</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2636,15 +2636,15 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>3.69</v>
+        <v>4.09</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>29/07/2023 18:58</t>
+          <t>29/07/2023 18:13</t>
         </is>
       </c>
       <c r="R24" t="n">
-        <v>3.65</v>
+        <v>5.22</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2652,16 +2652,16 @@
         </is>
       </c>
       <c r="T24" t="n">
-        <v>3.16</v>
+        <v>6.42</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>29/07/2023 18:58</t>
+          <t>29/07/2023 18:13</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/belasitsa-petrich-chernomorets-1919/vZsHGQu7/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-chernomorets-balchik/2VNpW5uf/</t>
         </is>
       </c>
     </row>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Belasitsa</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -2697,14 +2697,14 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>1.5</v>
+        <v>1.92</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -2712,15 +2712,15 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>1.42</v>
+        <v>1.93</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>29/07/2023 18:03</t>
+          <t>29/07/2023 18:58</t>
         </is>
       </c>
       <c r="N25" t="n">
-        <v>3.96</v>
+        <v>3.07</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2728,15 +2728,15 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>4.09</v>
+        <v>3.69</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>29/07/2023 18:13</t>
+          <t>29/07/2023 18:58</t>
         </is>
       </c>
       <c r="R25" t="n">
-        <v>5.22</v>
+        <v>3.65</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
@@ -2744,16 +2744,16 @@
         </is>
       </c>
       <c r="T25" t="n">
-        <v>6.42</v>
+        <v>3.16</v>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>29/07/2023 18:13</t>
+          <t>29/07/2023 18:58</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-chernomorets-balchik/2VNpW5uf/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/belasitsa-petrich-chernomorets-1919/vZsHGQu7/</t>
         </is>
       </c>
     </row>
@@ -3241,22 +3241,22 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Yantra Gabrovo</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="I31" t="n">
         <v>1</v>
       </c>
       <c r="J31" t="n">
-        <v>1.55</v>
+        <v>2.09</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -3264,15 +3264,15 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>1.79</v>
+        <v>1.99</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>05/08/2023 16:39</t>
+          <t>05/08/2023 16:45</t>
         </is>
       </c>
       <c r="N31" t="n">
-        <v>3.5</v>
+        <v>2.89</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -3280,15 +3280,15 @@
         </is>
       </c>
       <c r="P31" t="n">
-        <v>3.24</v>
+        <v>3.01</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>05/08/2023 16:39</t>
+          <t>05/08/2023 16:45</t>
         </is>
       </c>
       <c r="R31" t="n">
-        <v>4.58</v>
+        <v>3.1</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
@@ -3296,16 +3296,16 @@
         </is>
       </c>
       <c r="T31" t="n">
-        <v>4.19</v>
+        <v>3.68</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>05/08/2023 16:39</t>
+          <t>05/08/2023 16:45</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/yantra-gabrovo-maritsa-plovdiv/4bpGoous/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-dunav-ruse/nJcljRWP/</t>
         </is>
       </c>
     </row>
@@ -3333,22 +3333,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Yantra Gabrovo</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="I32" t="n">
         <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>2.09</v>
+        <v>1.55</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -3356,15 +3356,15 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>1.99</v>
+        <v>1.79</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>05/08/2023 16:45</t>
+          <t>05/08/2023 16:39</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>2.89</v>
+        <v>3.5</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3372,15 +3372,15 @@
         </is>
       </c>
       <c r="P32" t="n">
-        <v>3.01</v>
+        <v>3.24</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>05/08/2023 16:45</t>
+          <t>05/08/2023 16:39</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>3.1</v>
+        <v>4.58</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
@@ -3388,16 +3388,16 @@
         </is>
       </c>
       <c r="T32" t="n">
-        <v>3.68</v>
+        <v>4.19</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>05/08/2023 16:45</t>
+          <t>05/08/2023 16:39</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-dunav-ruse/nJcljRWP/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/yantra-gabrovo-maritsa-plovdiv/4bpGoous/</t>
         </is>
       </c>
     </row>
@@ -3793,71 +3793,71 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Yantra Gabrovo</t>
         </is>
       </c>
       <c r="I37" t="n">
         <v>3</v>
       </c>
       <c r="J37" t="n">
-        <v>1.61</v>
+        <v>1.87</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>13/08/2023 10:13</t>
+          <t>12/08/2023 05:12</t>
         </is>
       </c>
       <c r="L37" t="n">
-        <v>1.68</v>
+        <v>1.65</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>13/08/2023 16:52</t>
+          <t>13/08/2023 16:57</t>
         </is>
       </c>
       <c r="N37" t="n">
-        <v>3.51</v>
+        <v>2.94</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>13/08/2023 10:13</t>
+          <t>12/08/2023 05:12</t>
         </is>
       </c>
       <c r="P37" t="n">
-        <v>3.93</v>
+        <v>3.27</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>13/08/2023 16:52</t>
+          <t>13/08/2023 16:58</t>
         </is>
       </c>
       <c r="R37" t="n">
-        <v>4.84</v>
+        <v>3.66</v>
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>13/08/2023 10:13</t>
+          <t>12/08/2023 05:12</t>
         </is>
       </c>
       <c r="T37" t="n">
-        <v>3.87</v>
+        <v>5.21</v>
       </c>
       <c r="U37" t="inlineStr">
         <is>
-          <t>13/08/2023 16:52</t>
+          <t>13/08/2023 16:58</t>
         </is>
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-chernomorets-1919/pEuysNgC/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-yantra-gabrovo/SxVuts9I/</t>
         </is>
       </c>
     </row>
@@ -3977,71 +3977,71 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Yantra Gabrovo</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="I39" t="n">
         <v>3</v>
       </c>
       <c r="J39" t="n">
-        <v>1.87</v>
+        <v>1.61</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>12/08/2023 05:12</t>
+          <t>13/08/2023 10:13</t>
         </is>
       </c>
       <c r="L39" t="n">
-        <v>1.65</v>
+        <v>1.68</v>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>13/08/2023 16:57</t>
+          <t>13/08/2023 16:52</t>
         </is>
       </c>
       <c r="N39" t="n">
-        <v>2.94</v>
+        <v>3.51</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>12/08/2023 05:12</t>
+          <t>13/08/2023 10:13</t>
         </is>
       </c>
       <c r="P39" t="n">
-        <v>3.27</v>
+        <v>3.93</v>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>13/08/2023 16:58</t>
+          <t>13/08/2023 16:52</t>
         </is>
       </c>
       <c r="R39" t="n">
-        <v>3.66</v>
+        <v>4.84</v>
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>12/08/2023 05:12</t>
+          <t>13/08/2023 10:13</t>
         </is>
       </c>
       <c r="T39" t="n">
-        <v>5.21</v>
+        <v>3.87</v>
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>13/08/2023 16:58</t>
+          <t>13/08/2023 16:52</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-yantra-gabrovo/SxVuts9I/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-chernomorets-1919/pEuysNgC/</t>
         </is>
       </c>
     </row>
@@ -7105,22 +7105,22 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="I73" t="n">
         <v>0</v>
       </c>
       <c r="J73" t="n">
-        <v>3.17</v>
+        <v>1.27</v>
       </c>
       <c r="K73" t="inlineStr">
         <is>
@@ -7128,15 +7128,15 @@
         </is>
       </c>
       <c r="L73" t="n">
-        <v>2.61</v>
+        <v>1.2</v>
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>17/09/2023 15:49</t>
+          <t>17/09/2023 15:56</t>
         </is>
       </c>
       <c r="N73" t="n">
-        <v>2.89</v>
+        <v>4.38</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -7144,15 +7144,15 @@
         </is>
       </c>
       <c r="P73" t="n">
-        <v>2.98</v>
+        <v>5.25</v>
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>17/09/2023 15:49</t>
+          <t>17/09/2023 15:56</t>
         </is>
       </c>
       <c r="R73" t="n">
-        <v>2.06</v>
+        <v>7.61</v>
       </c>
       <c r="S73" t="inlineStr">
         <is>
@@ -7160,16 +7160,16 @@
         </is>
       </c>
       <c r="T73" t="n">
-        <v>2.6</v>
+        <v>13.6</v>
       </c>
       <c r="U73" t="inlineStr">
         <is>
-          <t>17/09/2023 15:49</t>
+          <t>17/09/2023 15:56</t>
         </is>
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-svoge/htdsF75e/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-bdin-vidin/r767L9SR/</t>
         </is>
       </c>
     </row>
@@ -7197,22 +7197,22 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Spartak Varna</t>
         </is>
       </c>
       <c r="I74" t="n">
         <v>1</v>
       </c>
       <c r="J74" t="n">
-        <v>1.75</v>
+        <v>2.56</v>
       </c>
       <c r="K74" t="inlineStr">
         <is>
@@ -7220,15 +7220,15 @@
         </is>
       </c>
       <c r="L74" t="n">
-        <v>1.75</v>
+        <v>3.02</v>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>17/09/2023 15:09</t>
+          <t>17/09/2023 15:46</t>
         </is>
       </c>
       <c r="N74" t="n">
-        <v>3.17</v>
+        <v>2.73</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -7236,15 +7236,15 @@
         </is>
       </c>
       <c r="P74" t="n">
-        <v>3.18</v>
+        <v>2.66</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>17/09/2023 15:23</t>
+          <t>17/09/2023 15:46</t>
         </is>
       </c>
       <c r="R74" t="n">
-        <v>3.84</v>
+        <v>2.63</v>
       </c>
       <c r="S74" t="inlineStr">
         <is>
@@ -7252,16 +7252,16 @@
         </is>
       </c>
       <c r="T74" t="n">
-        <v>4.58</v>
+        <v>2.52</v>
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>17/09/2023 15:08</t>
+          <t>17/09/2023 15:46</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-chernomorets-1919/KScZGTzq/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-spartak-varna/MiIbNVcF/</t>
         </is>
       </c>
     </row>
@@ -7289,22 +7289,22 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Ludogorets II</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="G75" t="n">
+        <v>2</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Svoge</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
         <v>0</v>
       </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>Spartak Pleven</t>
-        </is>
-      </c>
-      <c r="I75" t="n">
-        <v>2</v>
-      </c>
       <c r="J75" t="n">
-        <v>1.55</v>
+        <v>3.17</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
@@ -7312,15 +7312,15 @@
         </is>
       </c>
       <c r="L75" t="n">
-        <v>1.61</v>
+        <v>2.61</v>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>17/09/2023 15:57</t>
+          <t>17/09/2023 15:49</t>
         </is>
       </c>
       <c r="N75" t="n">
-        <v>3.54</v>
+        <v>2.89</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -7328,15 +7328,15 @@
         </is>
       </c>
       <c r="P75" t="n">
-        <v>3.49</v>
+        <v>2.98</v>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>17/09/2023 15:57</t>
+          <t>17/09/2023 15:49</t>
         </is>
       </c>
       <c r="R75" t="n">
-        <v>4.49</v>
+        <v>2.06</v>
       </c>
       <c r="S75" t="inlineStr">
         <is>
@@ -7344,16 +7344,16 @@
         </is>
       </c>
       <c r="T75" t="n">
-        <v>4.09</v>
+        <v>2.6</v>
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>17/09/2023 15:57</t>
+          <t>17/09/2023 15:49</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-spartak-pleven/bgRsDoz8/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-svoge/htdsF75e/</t>
         </is>
       </c>
     </row>
@@ -7381,22 +7381,22 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="G76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Spartak Varna</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="I76" t="n">
         <v>1</v>
       </c>
       <c r="J76" t="n">
-        <v>2.56</v>
+        <v>1.75</v>
       </c>
       <c r="K76" t="inlineStr">
         <is>
@@ -7404,15 +7404,15 @@
         </is>
       </c>
       <c r="L76" t="n">
-        <v>3.02</v>
+        <v>1.75</v>
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>17/09/2023 15:46</t>
+          <t>17/09/2023 15:09</t>
         </is>
       </c>
       <c r="N76" t="n">
-        <v>2.73</v>
+        <v>3.17</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -7420,15 +7420,15 @@
         </is>
       </c>
       <c r="P76" t="n">
-        <v>2.66</v>
+        <v>3.18</v>
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>17/09/2023 15:46</t>
+          <t>17/09/2023 15:23</t>
         </is>
       </c>
       <c r="R76" t="n">
-        <v>2.63</v>
+        <v>3.84</v>
       </c>
       <c r="S76" t="inlineStr">
         <is>
@@ -7436,16 +7436,16 @@
         </is>
       </c>
       <c r="T76" t="n">
-        <v>2.52</v>
+        <v>4.58</v>
       </c>
       <c r="U76" t="inlineStr">
         <is>
-          <t>17/09/2023 15:46</t>
+          <t>17/09/2023 15:08</t>
         </is>
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-spartak-varna/MiIbNVcF/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-chernomorets-1919/KScZGTzq/</t>
         </is>
       </c>
     </row>
@@ -7473,22 +7473,22 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Ludogorets II</t>
         </is>
       </c>
       <c r="G77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="I77" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J77" t="n">
-        <v>1.27</v>
+        <v>1.55</v>
       </c>
       <c r="K77" t="inlineStr">
         <is>
@@ -7496,15 +7496,15 @@
         </is>
       </c>
       <c r="L77" t="n">
-        <v>1.2</v>
+        <v>1.61</v>
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>17/09/2023 15:56</t>
+          <t>17/09/2023 15:57</t>
         </is>
       </c>
       <c r="N77" t="n">
-        <v>4.38</v>
+        <v>3.54</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -7512,15 +7512,15 @@
         </is>
       </c>
       <c r="P77" t="n">
-        <v>5.25</v>
+        <v>3.49</v>
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>17/09/2023 15:56</t>
+          <t>17/09/2023 15:57</t>
         </is>
       </c>
       <c r="R77" t="n">
-        <v>7.61</v>
+        <v>4.49</v>
       </c>
       <c r="S77" t="inlineStr">
         <is>
@@ -7528,16 +7528,16 @@
         </is>
       </c>
       <c r="T77" t="n">
-        <v>13.6</v>
+        <v>4.09</v>
       </c>
       <c r="U77" t="inlineStr">
         <is>
-          <t>17/09/2023 15:56</t>
+          <t>17/09/2023 15:57</t>
         </is>
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-bdin-vidin/r767L9SR/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-spartak-pleven/bgRsDoz8/</t>
         </is>
       </c>
     </row>
@@ -7933,22 +7933,22 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="I82" t="n">
         <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>2.38</v>
+        <v>1.55</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
@@ -7956,15 +7956,15 @@
         </is>
       </c>
       <c r="L82" t="n">
-        <v>2.33</v>
+        <v>1.95</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>22/09/2023 15:59</t>
+          <t>22/09/2023 15:56</t>
         </is>
       </c>
       <c r="N82" t="n">
-        <v>2.93</v>
+        <v>3.45</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -7972,15 +7972,15 @@
         </is>
       </c>
       <c r="P82" t="n">
-        <v>2.97</v>
+        <v>3.51</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>22/09/2023 15:59</t>
+          <t>22/09/2023 15:56</t>
         </is>
       </c>
       <c r="R82" t="n">
-        <v>2.6</v>
+        <v>4.66</v>
       </c>
       <c r="S82" t="inlineStr">
         <is>
@@ -7988,16 +7988,16 @@
         </is>
       </c>
       <c r="T82" t="n">
-        <v>2.96</v>
+        <v>3.24</v>
       </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>22/09/2023 15:59</t>
+          <t>22/09/2023 15:56</t>
         </is>
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-dunav-ruse/6JjLQ447/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-spartak-pleven/CdFPyVC8/</t>
         </is>
       </c>
     </row>
@@ -8025,22 +8025,22 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="I83" t="n">
         <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>1.55</v>
+        <v>2.38</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -8048,15 +8048,15 @@
         </is>
       </c>
       <c r="L83" t="n">
-        <v>1.95</v>
+        <v>2.33</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>22/09/2023 15:56</t>
+          <t>22/09/2023 15:59</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>3.45</v>
+        <v>2.93</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -8064,15 +8064,15 @@
         </is>
       </c>
       <c r="P83" t="n">
-        <v>3.51</v>
+        <v>2.97</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>22/09/2023 15:56</t>
+          <t>22/09/2023 15:59</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>4.66</v>
+        <v>2.6</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
@@ -8080,16 +8080,16 @@
         </is>
       </c>
       <c r="T83" t="n">
-        <v>3.24</v>
+        <v>2.96</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>22/09/2023 15:56</t>
+          <t>22/09/2023 15:59</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-spartak-pleven/CdFPyVC8/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-dunav-ruse/6JjLQ447/</t>
         </is>
       </c>
     </row>
@@ -11245,22 +11245,22 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="G118" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Ludogorets II</t>
         </is>
       </c>
       <c r="I118" t="n">
         <v>2</v>
       </c>
       <c r="J118" t="n">
-        <v>2.26</v>
+        <v>2.75</v>
       </c>
       <c r="K118" t="inlineStr">
         <is>
@@ -11268,15 +11268,15 @@
         </is>
       </c>
       <c r="L118" t="n">
-        <v>2.44</v>
+        <v>2.71</v>
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>21/10/2023 14:48</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="N118" t="n">
-        <v>2.88</v>
+        <v>2.81</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -11284,15 +11284,15 @@
         </is>
       </c>
       <c r="P118" t="n">
-        <v>2.83</v>
+        <v>2.85</v>
       </c>
       <c r="Q118" t="inlineStr">
         <is>
-          <t>21/10/2023 14:48</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="R118" t="n">
-        <v>2.8</v>
+        <v>2.34</v>
       </c>
       <c r="S118" t="inlineStr">
         <is>
@@ -11300,16 +11300,16 @@
         </is>
       </c>
       <c r="T118" t="n">
-        <v>2.93</v>
+        <v>2.6</v>
       </c>
       <c r="U118" t="inlineStr">
         <is>
-          <t>21/10/2023 14:48</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="V118" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-montana/MifLqvSq/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-ludogorets/OGEpjtkG/</t>
         </is>
       </c>
     </row>
@@ -11337,22 +11337,22 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="G119" t="n">
+        <v>3</v>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>Spartak Pleven</t>
+        </is>
+      </c>
+      <c r="I119" t="n">
         <v>0</v>
       </c>
-      <c r="H119" t="inlineStr">
-        <is>
-          <t>Ludogorets II</t>
-        </is>
-      </c>
-      <c r="I119" t="n">
-        <v>2</v>
-      </c>
       <c r="J119" t="n">
-        <v>2.75</v>
+        <v>1.88</v>
       </c>
       <c r="K119" t="inlineStr">
         <is>
@@ -11360,15 +11360,15 @@
         </is>
       </c>
       <c r="L119" t="n">
-        <v>2.71</v>
+        <v>1.59</v>
       </c>
       <c r="M119" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 14:51</t>
         </is>
       </c>
       <c r="N119" t="n">
-        <v>2.81</v>
+        <v>3.03</v>
       </c>
       <c r="O119" t="inlineStr">
         <is>
@@ -11376,15 +11376,15 @@
         </is>
       </c>
       <c r="P119" t="n">
-        <v>2.85</v>
+        <v>3.42</v>
       </c>
       <c r="Q119" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 14:51</t>
         </is>
       </c>
       <c r="R119" t="n">
-        <v>2.34</v>
+        <v>3.48</v>
       </c>
       <c r="S119" t="inlineStr">
         <is>
@@ -11392,16 +11392,16 @@
         </is>
       </c>
       <c r="T119" t="n">
-        <v>2.6</v>
+        <v>5.4</v>
       </c>
       <c r="U119" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 14:51</t>
         </is>
       </c>
       <c r="V119" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-ludogorets/OGEpjtkG/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-1919-spartak-pleven/UgFtiMZ9/</t>
         </is>
       </c>
     </row>
@@ -11429,22 +11429,22 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="G120" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="I120" t="n">
         <v>0</v>
       </c>
       <c r="J120" t="n">
-        <v>1.88</v>
+        <v>1.89</v>
       </c>
       <c r="K120" t="inlineStr">
         <is>
@@ -11452,15 +11452,15 @@
         </is>
       </c>
       <c r="L120" t="n">
-        <v>1.59</v>
+        <v>1.81</v>
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>21/10/2023 14:51</t>
+          <t>21/10/2023 14:54</t>
         </is>
       </c>
       <c r="N120" t="n">
-        <v>3.03</v>
+        <v>2.94</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -11468,15 +11468,15 @@
         </is>
       </c>
       <c r="P120" t="n">
-        <v>3.42</v>
+        <v>3.18</v>
       </c>
       <c r="Q120" t="inlineStr">
         <is>
-          <t>21/10/2023 14:51</t>
+          <t>21/10/2023 14:54</t>
         </is>
       </c>
       <c r="R120" t="n">
-        <v>3.48</v>
+        <v>3.71</v>
       </c>
       <c r="S120" t="inlineStr">
         <is>
@@ -11484,16 +11484,16 @@
         </is>
       </c>
       <c r="T120" t="n">
-        <v>5.4</v>
+        <v>4.22</v>
       </c>
       <c r="U120" t="inlineStr">
         <is>
-          <t>21/10/2023 14:51</t>
+          <t>21/10/2023 14:54</t>
         </is>
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-1919-spartak-pleven/UgFtiMZ9/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-svoge/zeMXhr5c/</t>
         </is>
       </c>
     </row>
@@ -11521,22 +11521,22 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="G121" t="n">
+        <v>1</v>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Montana</t>
+        </is>
+      </c>
+      <c r="I121" t="n">
         <v>2</v>
       </c>
-      <c r="H121" t="inlineStr">
-        <is>
-          <t>Svoge</t>
-        </is>
-      </c>
-      <c r="I121" t="n">
-        <v>0</v>
-      </c>
       <c r="J121" t="n">
-        <v>1.89</v>
+        <v>2.26</v>
       </c>
       <c r="K121" t="inlineStr">
         <is>
@@ -11544,15 +11544,15 @@
         </is>
       </c>
       <c r="L121" t="n">
-        <v>1.81</v>
+        <v>2.44</v>
       </c>
       <c r="M121" t="inlineStr">
         <is>
-          <t>21/10/2023 14:54</t>
+          <t>21/10/2023 14:48</t>
         </is>
       </c>
       <c r="N121" t="n">
-        <v>2.94</v>
+        <v>2.88</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -11560,15 +11560,15 @@
         </is>
       </c>
       <c r="P121" t="n">
-        <v>3.18</v>
+        <v>2.83</v>
       </c>
       <c r="Q121" t="inlineStr">
         <is>
-          <t>21/10/2023 14:54</t>
+          <t>21/10/2023 14:48</t>
         </is>
       </c>
       <c r="R121" t="n">
-        <v>3.71</v>
+        <v>2.8</v>
       </c>
       <c r="S121" t="inlineStr">
         <is>
@@ -11576,16 +11576,16 @@
         </is>
       </c>
       <c r="T121" t="n">
-        <v>4.22</v>
+        <v>2.93</v>
       </c>
       <c r="U121" t="inlineStr">
         <is>
-          <t>21/10/2023 14:54</t>
+          <t>21/10/2023 14:48</t>
         </is>
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-svoge/zeMXhr5c/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-montana/MifLqvSq/</t>
         </is>
       </c>
     </row>
@@ -11981,22 +11981,22 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="G126" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Septemvri Sofia</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="I126" t="n">
         <v>0</v>
       </c>
       <c r="J126" t="n">
-        <v>3.35</v>
+        <v>2.39</v>
       </c>
       <c r="K126" t="inlineStr">
         <is>
@@ -12004,15 +12004,15 @@
         </is>
       </c>
       <c r="L126" t="n">
-        <v>3.78</v>
+        <v>2.07</v>
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>27/10/2023 14:50</t>
+          <t>27/10/2023 14:51</t>
         </is>
       </c>
       <c r="N126" t="n">
-        <v>2.93</v>
+        <v>2.92</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -12020,15 +12020,15 @@
         </is>
       </c>
       <c r="P126" t="n">
-        <v>3.4</v>
+        <v>3.23</v>
       </c>
       <c r="Q126" t="inlineStr">
         <is>
-          <t>27/10/2023 14:50</t>
+          <t>27/10/2023 14:51</t>
         </is>
       </c>
       <c r="R126" t="n">
-        <v>1.95</v>
+        <v>2.59</v>
       </c>
       <c r="S126" t="inlineStr">
         <is>
@@ -12036,16 +12036,16 @@
         </is>
       </c>
       <c r="T126" t="n">
-        <v>1.83</v>
+        <v>3.2</v>
       </c>
       <c r="U126" t="inlineStr">
         <is>
-          <t>27/10/2023 14:50</t>
+          <t>27/10/2023 14:51</t>
         </is>
       </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-septemvri-sofia/ADzG5Ll3/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-maritsa-plovdiv/rulN3aJF/</t>
         </is>
       </c>
     </row>
@@ -12073,7 +12073,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>CSKA 1948 Sofia II</t>
         </is>
       </c>
       <c r="G127" t="n">
@@ -12081,14 +12081,14 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="I127" t="n">
         <v>0</v>
       </c>
       <c r="J127" t="n">
-        <v>2.39</v>
+        <v>1.46</v>
       </c>
       <c r="K127" t="inlineStr">
         <is>
@@ -12096,15 +12096,15 @@
         </is>
       </c>
       <c r="L127" t="n">
-        <v>2.07</v>
+        <v>1.51</v>
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>27/10/2023 14:51</t>
+          <t>27/10/2023 14:53</t>
         </is>
       </c>
       <c r="N127" t="n">
-        <v>2.92</v>
+        <v>3.67</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -12112,15 +12112,15 @@
         </is>
       </c>
       <c r="P127" t="n">
-        <v>3.23</v>
+        <v>3.64</v>
       </c>
       <c r="Q127" t="inlineStr">
         <is>
-          <t>27/10/2023 14:51</t>
+          <t>27/10/2023 14:53</t>
         </is>
       </c>
       <c r="R127" t="n">
-        <v>2.59</v>
+        <v>5.19</v>
       </c>
       <c r="S127" t="inlineStr">
         <is>
@@ -12128,16 +12128,16 @@
         </is>
       </c>
       <c r="T127" t="n">
-        <v>3.2</v>
+        <v>5.9</v>
       </c>
       <c r="U127" t="inlineStr">
         <is>
-          <t>27/10/2023 14:51</t>
+          <t>27/10/2023 14:53</t>
         </is>
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-maritsa-plovdiv/rulN3aJF/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/cska-1948-sofia-chernomorets-1919/Ag43qVX0/</t>
         </is>
       </c>
     </row>
@@ -12165,22 +12165,22 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>CSKA 1948 Sofia II</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="G128" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="I128" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J128" t="n">
-        <v>1.46</v>
+        <v>1.54</v>
       </c>
       <c r="K128" t="inlineStr">
         <is>
@@ -12188,7 +12188,7 @@
         </is>
       </c>
       <c r="L128" t="n">
-        <v>1.51</v>
+        <v>1.42</v>
       </c>
       <c r="M128" t="inlineStr">
         <is>
@@ -12196,7 +12196,7 @@
         </is>
       </c>
       <c r="N128" t="n">
-        <v>3.67</v>
+        <v>3.39</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -12204,7 +12204,7 @@
         </is>
       </c>
       <c r="P128" t="n">
-        <v>3.64</v>
+        <v>3.83</v>
       </c>
       <c r="Q128" t="inlineStr">
         <is>
@@ -12212,7 +12212,7 @@
         </is>
       </c>
       <c r="R128" t="n">
-        <v>5.19</v>
+        <v>4.81</v>
       </c>
       <c r="S128" t="inlineStr">
         <is>
@@ -12220,7 +12220,7 @@
         </is>
       </c>
       <c r="T128" t="n">
-        <v>5.9</v>
+        <v>7.25</v>
       </c>
       <c r="U128" t="inlineStr">
         <is>
@@ -12229,7 +12229,7 @@
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/cska-1948-sofia-chernomorets-1919/Ag43qVX0/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-marek/WMyC61Zd/</t>
         </is>
       </c>
     </row>
@@ -12257,22 +12257,22 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Ludogorets II</t>
         </is>
       </c>
       <c r="G129" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Belasitsa</t>
         </is>
       </c>
       <c r="I129" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J129" t="n">
-        <v>1.54</v>
+        <v>1.68</v>
       </c>
       <c r="K129" t="inlineStr">
         <is>
@@ -12280,15 +12280,15 @@
         </is>
       </c>
       <c r="L129" t="n">
-        <v>1.42</v>
+        <v>1.6</v>
       </c>
       <c r="M129" t="inlineStr">
         <is>
-          <t>27/10/2023 14:53</t>
+          <t>27/10/2023 13:03</t>
         </is>
       </c>
       <c r="N129" t="n">
-        <v>3.39</v>
+        <v>3.24</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -12296,15 +12296,15 @@
         </is>
       </c>
       <c r="P129" t="n">
-        <v>3.83</v>
+        <v>3.51</v>
       </c>
       <c r="Q129" t="inlineStr">
         <is>
-          <t>27/10/2023 14:53</t>
+          <t>27/10/2023 13:41</t>
         </is>
       </c>
       <c r="R129" t="n">
-        <v>4.81</v>
+        <v>4.05</v>
       </c>
       <c r="S129" t="inlineStr">
         <is>
@@ -12312,16 +12312,16 @@
         </is>
       </c>
       <c r="T129" t="n">
-        <v>7.25</v>
+        <v>5.13</v>
       </c>
       <c r="U129" t="inlineStr">
         <is>
-          <t>27/10/2023 14:53</t>
+          <t>27/10/2023 13:03</t>
         </is>
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-marek/WMyC61Zd/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-belasitsa-petrich/xt6eoi3l/</t>
         </is>
       </c>
     </row>
@@ -12349,22 +12349,22 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Ludogorets II</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="G130" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>Belasitsa</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="I130" t="n">
         <v>1</v>
       </c>
       <c r="J130" t="n">
-        <v>1.68</v>
+        <v>2</v>
       </c>
       <c r="K130" t="inlineStr">
         <is>
@@ -12372,15 +12372,15 @@
         </is>
       </c>
       <c r="L130" t="n">
-        <v>1.6</v>
+        <v>1.85</v>
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>27/10/2023 13:03</t>
+          <t>27/10/2023 14:48</t>
         </is>
       </c>
       <c r="N130" t="n">
-        <v>3.24</v>
+        <v>2.86</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -12388,15 +12388,15 @@
         </is>
       </c>
       <c r="P130" t="n">
-        <v>3.51</v>
+        <v>2.88</v>
       </c>
       <c r="Q130" t="inlineStr">
         <is>
-          <t>27/10/2023 13:41</t>
+          <t>27/10/2023 14:48</t>
         </is>
       </c>
       <c r="R130" t="n">
-        <v>4.05</v>
+        <v>3.34</v>
       </c>
       <c r="S130" t="inlineStr">
         <is>
@@ -12404,16 +12404,16 @@
         </is>
       </c>
       <c r="T130" t="n">
-        <v>5.13</v>
+        <v>4.6</v>
       </c>
       <c r="U130" t="inlineStr">
         <is>
-          <t>27/10/2023 13:03</t>
+          <t>27/10/2023 14:48</t>
         </is>
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-belasitsa-petrich/xt6eoi3l/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-dunav-ruse/4lkJ4u49/</t>
         </is>
       </c>
     </row>
@@ -12441,7 +12441,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="G131" t="n">
@@ -12449,14 +12449,14 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="I131" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J131" t="n">
-        <v>2</v>
+        <v>1.66</v>
       </c>
       <c r="K131" t="inlineStr">
         <is>
@@ -12464,15 +12464,15 @@
         </is>
       </c>
       <c r="L131" t="n">
-        <v>1.85</v>
+        <v>1.62</v>
       </c>
       <c r="M131" t="inlineStr">
         <is>
-          <t>27/10/2023 14:48</t>
+          <t>27/10/2023 14:53</t>
         </is>
       </c>
       <c r="N131" t="n">
-        <v>2.86</v>
+        <v>3.2</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -12480,15 +12480,15 @@
         </is>
       </c>
       <c r="P131" t="n">
-        <v>2.88</v>
+        <v>3.21</v>
       </c>
       <c r="Q131" t="inlineStr">
         <is>
-          <t>27/10/2023 14:48</t>
+          <t>27/10/2023 14:53</t>
         </is>
       </c>
       <c r="R131" t="n">
-        <v>3.34</v>
+        <v>4.24</v>
       </c>
       <c r="S131" t="inlineStr">
         <is>
@@ -12496,16 +12496,16 @@
         </is>
       </c>
       <c r="T131" t="n">
-        <v>4.6</v>
+        <v>5.62</v>
       </c>
       <c r="U131" t="inlineStr">
         <is>
-          <t>27/10/2023 14:48</t>
+          <t>27/10/2023 14:51</t>
         </is>
       </c>
       <c r="V131" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-dunav-ruse/4lkJ4u49/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-bdin-vidin/W25apBIf/</t>
         </is>
       </c>
     </row>
@@ -12533,7 +12533,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="G132" t="n">
@@ -12541,14 +12541,14 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Septemvri Sofia</t>
         </is>
       </c>
       <c r="I132" t="n">
         <v>0</v>
       </c>
       <c r="J132" t="n">
-        <v>1.66</v>
+        <v>3.35</v>
       </c>
       <c r="K132" t="inlineStr">
         <is>
@@ -12556,15 +12556,15 @@
         </is>
       </c>
       <c r="L132" t="n">
-        <v>1.62</v>
+        <v>3.78</v>
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>27/10/2023 14:53</t>
+          <t>27/10/2023 14:50</t>
         </is>
       </c>
       <c r="N132" t="n">
-        <v>3.2</v>
+        <v>2.93</v>
       </c>
       <c r="O132" t="inlineStr">
         <is>
@@ -12572,15 +12572,15 @@
         </is>
       </c>
       <c r="P132" t="n">
-        <v>3.21</v>
+        <v>3.4</v>
       </c>
       <c r="Q132" t="inlineStr">
         <is>
-          <t>27/10/2023 14:53</t>
+          <t>27/10/2023 14:50</t>
         </is>
       </c>
       <c r="R132" t="n">
-        <v>4.24</v>
+        <v>1.95</v>
       </c>
       <c r="S132" t="inlineStr">
         <is>
@@ -12588,16 +12588,16 @@
         </is>
       </c>
       <c r="T132" t="n">
-        <v>5.62</v>
+        <v>1.83</v>
       </c>
       <c r="U132" t="inlineStr">
         <is>
-          <t>27/10/2023 14:51</t>
+          <t>27/10/2023 14:50</t>
         </is>
       </c>
       <c r="V132" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-bdin-vidin/W25apBIf/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-septemvri-sofia/ADzG5Ll3/</t>
         </is>
       </c>
     </row>
@@ -13821,22 +13821,22 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="G146" t="n">
+        <v>2</v>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Bdin Vidin</t>
+        </is>
+      </c>
+      <c r="I146" t="n">
         <v>0</v>
       </c>
-      <c r="H146" t="inlineStr">
-        <is>
-          <t>Septemvri Sofia</t>
-        </is>
-      </c>
-      <c r="I146" t="n">
-        <v>2</v>
-      </c>
       <c r="J146" t="n">
-        <v>5.09</v>
+        <v>1.64</v>
       </c>
       <c r="K146" t="inlineStr">
         <is>
@@ -13844,15 +13844,15 @@
         </is>
       </c>
       <c r="L146" t="n">
-        <v>6.24</v>
+        <v>1.56</v>
       </c>
       <c r="M146" t="inlineStr">
         <is>
-          <t>12/11/2023 13:15</t>
+          <t>12/11/2023 13:28</t>
         </is>
       </c>
       <c r="N146" t="n">
-        <v>3.54</v>
+        <v>3.34</v>
       </c>
       <c r="O146" t="inlineStr">
         <is>
@@ -13860,15 +13860,15 @@
         </is>
       </c>
       <c r="P146" t="n">
-        <v>3.84</v>
+        <v>3.44</v>
       </c>
       <c r="Q146" t="inlineStr">
         <is>
-          <t>12/11/2023 13:15</t>
+          <t>12/11/2023 13:28</t>
         </is>
       </c>
       <c r="R146" t="n">
-        <v>1.56</v>
+        <v>4.93</v>
       </c>
       <c r="S146" t="inlineStr">
         <is>
@@ -13876,16 +13876,16 @@
         </is>
       </c>
       <c r="T146" t="n">
-        <v>1.46</v>
+        <v>5.77</v>
       </c>
       <c r="U146" t="inlineStr">
         <is>
-          <t>12/11/2023 13:15</t>
+          <t>12/11/2023 13:28</t>
         </is>
       </c>
       <c r="V146" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-septemvri-sofia/hURUIVOJ/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-bdin-vidin/OI5DA7Wa/</t>
         </is>
       </c>
     </row>
@@ -13913,22 +13913,22 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>Litex Lovech</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="G147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Septemvri Sofia</t>
         </is>
       </c>
       <c r="I147" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J147" t="n">
-        <v>2.62</v>
+        <v>5.09</v>
       </c>
       <c r="K147" t="inlineStr">
         <is>
@@ -13936,15 +13936,15 @@
         </is>
       </c>
       <c r="L147" t="n">
-        <v>2.06</v>
+        <v>6.24</v>
       </c>
       <c r="M147" t="inlineStr">
         <is>
-          <t>12/11/2023 13:22</t>
+          <t>12/11/2023 13:15</t>
         </is>
       </c>
       <c r="N147" t="n">
-        <v>2.74</v>
+        <v>3.54</v>
       </c>
       <c r="O147" t="inlineStr">
         <is>
@@ -13952,15 +13952,15 @@
         </is>
       </c>
       <c r="P147" t="n">
-        <v>2.96</v>
+        <v>3.84</v>
       </c>
       <c r="Q147" t="inlineStr">
         <is>
-          <t>12/11/2023 13:22</t>
+          <t>12/11/2023 13:15</t>
         </is>
       </c>
       <c r="R147" t="n">
-        <v>2.75</v>
+        <v>1.56</v>
       </c>
       <c r="S147" t="inlineStr">
         <is>
@@ -13968,16 +13968,16 @@
         </is>
       </c>
       <c r="T147" t="n">
-        <v>3.54</v>
+        <v>1.46</v>
       </c>
       <c r="U147" t="inlineStr">
         <is>
-          <t>12/11/2023 13:22</t>
+          <t>12/11/2023 13:15</t>
         </is>
       </c>
       <c r="V147" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/litex-lovech-dunav-ruse/WKQYHkvQ/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-septemvri-sofia/hURUIVOJ/</t>
         </is>
       </c>
     </row>
@@ -14005,22 +14005,22 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Litex Lovech</t>
         </is>
       </c>
       <c r="G148" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>Spartak Varna</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="I148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J148" t="n">
-        <v>4.82</v>
+        <v>2.62</v>
       </c>
       <c r="K148" t="inlineStr">
         <is>
@@ -14028,15 +14028,15 @@
         </is>
       </c>
       <c r="L148" t="n">
-        <v>5.52</v>
+        <v>2.06</v>
       </c>
       <c r="M148" t="inlineStr">
         <is>
-          <t>12/11/2023 12:36</t>
+          <t>12/11/2023 13:22</t>
         </is>
       </c>
       <c r="N148" t="n">
-        <v>3.49</v>
+        <v>2.74</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -14044,15 +14044,15 @@
         </is>
       </c>
       <c r="P148" t="n">
-        <v>3.67</v>
+        <v>2.96</v>
       </c>
       <c r="Q148" t="inlineStr">
         <is>
-          <t>12/11/2023 12:36</t>
+          <t>12/11/2023 13:22</t>
         </is>
       </c>
       <c r="R148" t="n">
-        <v>1.59</v>
+        <v>2.75</v>
       </c>
       <c r="S148" t="inlineStr">
         <is>
@@ -14060,16 +14060,16 @@
         </is>
       </c>
       <c r="T148" t="n">
-        <v>1.53</v>
+        <v>3.54</v>
       </c>
       <c r="U148" t="inlineStr">
         <is>
-          <t>12/11/2023 12:36</t>
+          <t>12/11/2023 13:22</t>
         </is>
       </c>
       <c r="V148" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-spartak-varna/23H4CT1m/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/litex-lovech-dunav-ruse/WKQYHkvQ/</t>
         </is>
       </c>
     </row>
@@ -14097,22 +14097,22 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="G149" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Spartak Varna</t>
         </is>
       </c>
       <c r="I149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J149" t="n">
-        <v>2.09</v>
+        <v>4.82</v>
       </c>
       <c r="K149" t="inlineStr">
         <is>
@@ -14120,15 +14120,15 @@
         </is>
       </c>
       <c r="L149" t="n">
-        <v>1.8</v>
+        <v>5.52</v>
       </c>
       <c r="M149" t="inlineStr">
         <is>
-          <t>12/11/2023 13:06</t>
+          <t>12/11/2023 12:36</t>
         </is>
       </c>
       <c r="N149" t="n">
-        <v>2.93</v>
+        <v>3.49</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -14136,15 +14136,15 @@
         </is>
       </c>
       <c r="P149" t="n">
-        <v>3.09</v>
+        <v>3.67</v>
       </c>
       <c r="Q149" t="inlineStr">
         <is>
-          <t>12/11/2023 13:06</t>
+          <t>12/11/2023 12:36</t>
         </is>
       </c>
       <c r="R149" t="n">
-        <v>3.33</v>
+        <v>1.59</v>
       </c>
       <c r="S149" t="inlineStr">
         <is>
@@ -14152,16 +14152,16 @@
         </is>
       </c>
       <c r="T149" t="n">
-        <v>4.41</v>
+        <v>1.53</v>
       </c>
       <c r="U149" t="inlineStr">
         <is>
-          <t>12/11/2023 13:06</t>
+          <t>12/11/2023 12:36</t>
         </is>
       </c>
       <c r="V149" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-marek/EoNkeSWC/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-spartak-varna/23H4CT1m/</t>
         </is>
       </c>
     </row>
@@ -14189,22 +14189,22 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="G150" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="I150" t="n">
         <v>0</v>
       </c>
       <c r="J150" t="n">
-        <v>1.64</v>
+        <v>2.09</v>
       </c>
       <c r="K150" t="inlineStr">
         <is>
@@ -14212,15 +14212,15 @@
         </is>
       </c>
       <c r="L150" t="n">
-        <v>1.56</v>
+        <v>1.8</v>
       </c>
       <c r="M150" t="inlineStr">
         <is>
-          <t>12/11/2023 13:28</t>
+          <t>12/11/2023 13:06</t>
         </is>
       </c>
       <c r="N150" t="n">
-        <v>3.34</v>
+        <v>2.93</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -14228,15 +14228,15 @@
         </is>
       </c>
       <c r="P150" t="n">
-        <v>3.44</v>
+        <v>3.09</v>
       </c>
       <c r="Q150" t="inlineStr">
         <is>
-          <t>12/11/2023 13:28</t>
+          <t>12/11/2023 13:06</t>
         </is>
       </c>
       <c r="R150" t="n">
-        <v>4.93</v>
+        <v>3.33</v>
       </c>
       <c r="S150" t="inlineStr">
         <is>
@@ -14244,16 +14244,16 @@
         </is>
       </c>
       <c r="T150" t="n">
-        <v>5.77</v>
+        <v>4.41</v>
       </c>
       <c r="U150" t="inlineStr">
         <is>
-          <t>12/11/2023 13:28</t>
+          <t>12/11/2023 13:06</t>
         </is>
       </c>
       <c r="V150" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-bdin-vidin/OI5DA7Wa/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-marek/EoNkeSWC/</t>
         </is>
       </c>
     </row>
@@ -14557,71 +14557,71 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="G154" t="n">
+        <v>2</v>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>Maritsa Plovdiv</t>
+        </is>
+      </c>
+      <c r="I154" t="n">
         <v>0</v>
       </c>
-      <c r="H154" t="inlineStr">
-        <is>
-          <t>Strumska Slava</t>
-        </is>
-      </c>
-      <c r="I154" t="n">
-        <v>1</v>
-      </c>
       <c r="J154" t="n">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="K154" t="inlineStr">
         <is>
-          <t>25/11/2023 02:42</t>
+          <t>25/11/2023 02:43</t>
         </is>
       </c>
       <c r="L154" t="n">
-        <v>1.56</v>
+        <v>1.78</v>
       </c>
       <c r="M154" t="inlineStr">
         <is>
-          <t>25/11/2023 13:21</t>
+          <t>25/11/2023 13:27</t>
         </is>
       </c>
       <c r="N154" t="n">
-        <v>3.13</v>
+        <v>3.12</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
-          <t>25/11/2023 02:42</t>
+          <t>25/11/2023 02:43</t>
         </is>
       </c>
       <c r="P154" t="n">
-        <v>3.47</v>
+        <v>3.39</v>
       </c>
       <c r="Q154" t="inlineStr">
         <is>
-          <t>25/11/2023 13:21</t>
+          <t>25/11/2023 13:28</t>
         </is>
       </c>
       <c r="R154" t="n">
-        <v>3.82</v>
+        <v>3.34</v>
       </c>
       <c r="S154" t="inlineStr">
         <is>
-          <t>25/11/2023 02:42</t>
+          <t>25/11/2023 02:43</t>
         </is>
       </c>
       <c r="T154" t="n">
-        <v>5.74</v>
+        <v>4.02</v>
       </c>
       <c r="U154" t="inlineStr">
         <is>
-          <t>25/11/2023 13:21</t>
+          <t>25/11/2023 13:28</t>
         </is>
       </c>
       <c r="V154" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-strumska-slava/WdlfNpG5/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-maritsa-plovdiv/S4iwRSGt/</t>
         </is>
       </c>
     </row>
@@ -14649,71 +14649,71 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="G155" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Belasitsa</t>
         </is>
       </c>
       <c r="I155" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J155" t="n">
-        <v>2</v>
+        <v>1.71</v>
       </c>
       <c r="K155" t="inlineStr">
         <is>
-          <t>25/11/2023 02:43</t>
+          <t>25/11/2023 02:42</t>
         </is>
       </c>
       <c r="L155" t="n">
-        <v>1.78</v>
+        <v>2.19</v>
       </c>
       <c r="M155" t="inlineStr">
         <is>
-          <t>25/11/2023 13:27</t>
+          <t>25/11/2023 12:41</t>
         </is>
       </c>
       <c r="N155" t="n">
-        <v>3.12</v>
+        <v>3.26</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
-          <t>25/11/2023 02:43</t>
+          <t>25/11/2023 02:42</t>
         </is>
       </c>
       <c r="P155" t="n">
-        <v>3.39</v>
+        <v>2.76</v>
       </c>
       <c r="Q155" t="inlineStr">
         <is>
-          <t>25/11/2023 13:28</t>
+          <t>25/11/2023 12:41</t>
         </is>
       </c>
       <c r="R155" t="n">
-        <v>3.34</v>
+        <v>4.35</v>
       </c>
       <c r="S155" t="inlineStr">
         <is>
-          <t>25/11/2023 02:43</t>
+          <t>25/11/2023 02:42</t>
         </is>
       </c>
       <c r="T155" t="n">
-        <v>4.02</v>
+        <v>3.49</v>
       </c>
       <c r="U155" t="inlineStr">
         <is>
-          <t>25/11/2023 13:28</t>
+          <t>25/11/2023 12:41</t>
         </is>
       </c>
       <c r="V155" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-maritsa-plovdiv/S4iwRSGt/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-belasitsa-petrich/ChHT6PVO/</t>
         </is>
       </c>
     </row>
@@ -14833,22 +14833,22 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="G157" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>Belasitsa</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="I157" t="n">
         <v>1</v>
       </c>
       <c r="J157" t="n">
-        <v>1.71</v>
+        <v>1.85</v>
       </c>
       <c r="K157" t="inlineStr">
         <is>
@@ -14856,15 +14856,15 @@
         </is>
       </c>
       <c r="L157" t="n">
-        <v>2.19</v>
+        <v>1.56</v>
       </c>
       <c r="M157" t="inlineStr">
         <is>
-          <t>25/11/2023 12:41</t>
+          <t>25/11/2023 13:21</t>
         </is>
       </c>
       <c r="N157" t="n">
-        <v>3.26</v>
+        <v>3.13</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -14872,15 +14872,15 @@
         </is>
       </c>
       <c r="P157" t="n">
-        <v>2.76</v>
+        <v>3.47</v>
       </c>
       <c r="Q157" t="inlineStr">
         <is>
-          <t>25/11/2023 12:41</t>
+          <t>25/11/2023 13:21</t>
         </is>
       </c>
       <c r="R157" t="n">
-        <v>4.35</v>
+        <v>3.82</v>
       </c>
       <c r="S157" t="inlineStr">
         <is>
@@ -14888,16 +14888,108 @@
         </is>
       </c>
       <c r="T157" t="n">
-        <v>3.49</v>
+        <v>5.74</v>
       </c>
       <c r="U157" t="inlineStr">
         <is>
-          <t>25/11/2023 12:41</t>
+          <t>25/11/2023 13:21</t>
         </is>
       </c>
       <c r="V157" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-belasitsa-petrich/ChHT6PVO/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-strumska-slava/WdlfNpG5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>bulgaria</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>vtora-liga</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E158" s="2" t="n">
+        <v>45257.625</v>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Litex Lovech</t>
+        </is>
+      </c>
+      <c r="G158" t="n">
+        <v>1</v>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>Septemvri Sofia</t>
+        </is>
+      </c>
+      <c r="I158" t="n">
+        <v>0</v>
+      </c>
+      <c r="J158" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>27/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="L158" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>27/11/2023 14:23</t>
+        </is>
+      </c>
+      <c r="N158" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="O158" t="inlineStr">
+        <is>
+          <t>27/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P158" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="Q158" t="inlineStr">
+        <is>
+          <t>27/11/2023 14:24</t>
+        </is>
+      </c>
+      <c r="R158" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="S158" t="inlineStr">
+        <is>
+          <t>27/11/2023 03:12</t>
+        </is>
+      </c>
+      <c r="T158" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="U158" t="inlineStr">
+        <is>
+          <t>27/11/2023 14:24</t>
+        </is>
+      </c>
+      <c r="V158" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/litex-lovech-septemvri-sofia/OWpnP6og/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 29-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/bulgaria_vtora-liga_2023-2024.xlsx
+++ b/2023/bulgaria_vtora-liga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V158"/>
+  <dimension ref="A1:V159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14557,71 +14557,71 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="G154" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="I154" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J154" t="n">
-        <v>2</v>
+        <v>4.8</v>
       </c>
       <c r="K154" t="inlineStr">
         <is>
-          <t>25/11/2023 02:43</t>
+          <t>25/11/2023 02:42</t>
         </is>
       </c>
       <c r="L154" t="n">
-        <v>1.78</v>
+        <v>4.43</v>
       </c>
       <c r="M154" t="inlineStr">
         <is>
-          <t>25/11/2023 13:27</t>
+          <t>25/11/2023 12:46</t>
         </is>
       </c>
       <c r="N154" t="n">
-        <v>3.12</v>
+        <v>3.37</v>
       </c>
       <c r="O154" t="inlineStr">
         <is>
-          <t>25/11/2023 02:43</t>
+          <t>25/11/2023 02:42</t>
         </is>
       </c>
       <c r="P154" t="n">
-        <v>3.39</v>
+        <v>3.58</v>
       </c>
       <c r="Q154" t="inlineStr">
         <is>
-          <t>25/11/2023 13:28</t>
+          <t>25/11/2023 12:46</t>
         </is>
       </c>
       <c r="R154" t="n">
-        <v>3.34</v>
+        <v>1.62</v>
       </c>
       <c r="S154" t="inlineStr">
         <is>
-          <t>25/11/2023 02:43</t>
+          <t>25/11/2023 02:42</t>
         </is>
       </c>
       <c r="T154" t="n">
-        <v>4.02</v>
+        <v>1.66</v>
       </c>
       <c r="U154" t="inlineStr">
         <is>
-          <t>25/11/2023 13:28</t>
+          <t>25/11/2023 12:46</t>
         </is>
       </c>
       <c r="V154" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-maritsa-plovdiv/S4iwRSGt/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-dobrudzha/IgpjOQ0a/</t>
         </is>
       </c>
     </row>
@@ -14649,22 +14649,22 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="G155" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>Belasitsa</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="I155" t="n">
         <v>1</v>
       </c>
       <c r="J155" t="n">
-        <v>1.71</v>
+        <v>1.85</v>
       </c>
       <c r="K155" t="inlineStr">
         <is>
@@ -14672,15 +14672,15 @@
         </is>
       </c>
       <c r="L155" t="n">
-        <v>2.19</v>
+        <v>1.56</v>
       </c>
       <c r="M155" t="inlineStr">
         <is>
-          <t>25/11/2023 12:41</t>
+          <t>25/11/2023 13:21</t>
         </is>
       </c>
       <c r="N155" t="n">
-        <v>3.26</v>
+        <v>3.13</v>
       </c>
       <c r="O155" t="inlineStr">
         <is>
@@ -14688,15 +14688,15 @@
         </is>
       </c>
       <c r="P155" t="n">
-        <v>2.76</v>
+        <v>3.47</v>
       </c>
       <c r="Q155" t="inlineStr">
         <is>
-          <t>25/11/2023 12:41</t>
+          <t>25/11/2023 13:21</t>
         </is>
       </c>
       <c r="R155" t="n">
-        <v>4.35</v>
+        <v>3.82</v>
       </c>
       <c r="S155" t="inlineStr">
         <is>
@@ -14704,16 +14704,16 @@
         </is>
       </c>
       <c r="T155" t="n">
-        <v>3.49</v>
+        <v>5.74</v>
       </c>
       <c r="U155" t="inlineStr">
         <is>
-          <t>25/11/2023 12:41</t>
+          <t>25/11/2023 13:21</t>
         </is>
       </c>
       <c r="V155" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-belasitsa-petrich/ChHT6PVO/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-strumska-slava/WdlfNpG5/</t>
         </is>
       </c>
     </row>
@@ -14741,71 +14741,71 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="G156" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="I156" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J156" t="n">
-        <v>4.8</v>
+        <v>2</v>
       </c>
       <c r="K156" t="inlineStr">
         <is>
-          <t>25/11/2023 02:42</t>
+          <t>25/11/2023 02:43</t>
         </is>
       </c>
       <c r="L156" t="n">
-        <v>4.43</v>
+        <v>1.78</v>
       </c>
       <c r="M156" t="inlineStr">
         <is>
-          <t>25/11/2023 12:46</t>
+          <t>25/11/2023 13:27</t>
         </is>
       </c>
       <c r="N156" t="n">
-        <v>3.37</v>
+        <v>3.12</v>
       </c>
       <c r="O156" t="inlineStr">
         <is>
-          <t>25/11/2023 02:42</t>
+          <t>25/11/2023 02:43</t>
         </is>
       </c>
       <c r="P156" t="n">
-        <v>3.58</v>
+        <v>3.39</v>
       </c>
       <c r="Q156" t="inlineStr">
         <is>
-          <t>25/11/2023 12:46</t>
+          <t>25/11/2023 13:28</t>
         </is>
       </c>
       <c r="R156" t="n">
-        <v>1.62</v>
+        <v>3.34</v>
       </c>
       <c r="S156" t="inlineStr">
         <is>
-          <t>25/11/2023 02:42</t>
+          <t>25/11/2023 02:43</t>
         </is>
       </c>
       <c r="T156" t="n">
-        <v>1.66</v>
+        <v>4.02</v>
       </c>
       <c r="U156" t="inlineStr">
         <is>
-          <t>25/11/2023 12:46</t>
+          <t>25/11/2023 13:28</t>
         </is>
       </c>
       <c r="V156" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-dobrudzha/IgpjOQ0a/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-maritsa-plovdiv/S4iwRSGt/</t>
         </is>
       </c>
     </row>
@@ -14833,22 +14833,22 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="G157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Belasitsa</t>
         </is>
       </c>
       <c r="I157" t="n">
         <v>1</v>
       </c>
       <c r="J157" t="n">
-        <v>1.85</v>
+        <v>1.71</v>
       </c>
       <c r="K157" t="inlineStr">
         <is>
@@ -14856,15 +14856,15 @@
         </is>
       </c>
       <c r="L157" t="n">
-        <v>1.56</v>
+        <v>2.19</v>
       </c>
       <c r="M157" t="inlineStr">
         <is>
-          <t>25/11/2023 13:21</t>
+          <t>25/11/2023 12:41</t>
         </is>
       </c>
       <c r="N157" t="n">
-        <v>3.13</v>
+        <v>3.26</v>
       </c>
       <c r="O157" t="inlineStr">
         <is>
@@ -14872,15 +14872,15 @@
         </is>
       </c>
       <c r="P157" t="n">
-        <v>3.47</v>
+        <v>2.76</v>
       </c>
       <c r="Q157" t="inlineStr">
         <is>
-          <t>25/11/2023 13:21</t>
+          <t>25/11/2023 12:41</t>
         </is>
       </c>
       <c r="R157" t="n">
-        <v>3.82</v>
+        <v>4.35</v>
       </c>
       <c r="S157" t="inlineStr">
         <is>
@@ -14888,16 +14888,16 @@
         </is>
       </c>
       <c r="T157" t="n">
-        <v>5.74</v>
+        <v>3.49</v>
       </c>
       <c r="U157" t="inlineStr">
         <is>
-          <t>25/11/2023 13:21</t>
+          <t>25/11/2023 12:41</t>
         </is>
       </c>
       <c r="V157" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-strumska-slava/WdlfNpG5/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-belasitsa-petrich/ChHT6PVO/</t>
         </is>
       </c>
     </row>
@@ -14990,6 +14990,98 @@
       <c r="V158" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/litex-lovech-septemvri-sofia/OWpnP6og/</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>bulgaria</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>vtora-liga</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E159" s="2" t="n">
+        <v>45259.5625</v>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Marek</t>
+        </is>
+      </c>
+      <c r="G159" t="n">
+        <v>3</v>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>Chernomorets 1919</t>
+        </is>
+      </c>
+      <c r="I159" t="n">
+        <v>1</v>
+      </c>
+      <c r="J159" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>28/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="L159" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="M159" t="inlineStr">
+        <is>
+          <t>29/11/2023 13:00</t>
+        </is>
+      </c>
+      <c r="N159" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="O159" t="inlineStr">
+        <is>
+          <t>28/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="P159" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="Q159" t="inlineStr">
+        <is>
+          <t>29/11/2023 13:20</t>
+        </is>
+      </c>
+      <c r="R159" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="S159" t="inlineStr">
+        <is>
+          <t>28/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="T159" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="U159" t="inlineStr">
+        <is>
+          <t>29/11/2023 13:00</t>
+        </is>
+      </c>
+      <c r="V159" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-chernomorets-1919/Wr9L8o1C/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 01-12-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/bulgaria_vtora-liga_2023-2024.xlsx
+++ b/2023/bulgaria_vtora-liga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V159"/>
+  <dimension ref="A1:V160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1493,22 +1493,22 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>CSKA 1948 Sofia II</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>3.14</v>
+        <v>1.27</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -1516,15 +1516,15 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>3.17</v>
+        <v>1.49</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>22/07/2023 17:28</t>
+          <t>22/07/2023 17:27</t>
         </is>
       </c>
       <c r="N12" t="n">
-        <v>2.96</v>
+        <v>4.63</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1532,15 +1532,15 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>3.09</v>
+        <v>3.91</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>22/07/2023 17:28</t>
+          <t>22/07/2023 17:27</t>
         </is>
       </c>
       <c r="R12" t="n">
-        <v>2.04</v>
+        <v>6.8</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
@@ -1548,16 +1548,16 @@
         </is>
       </c>
       <c r="T12" t="n">
-        <v>2.14</v>
+        <v>5.61</v>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>22/07/2023 17:28</t>
+          <t>22/07/2023 17:27</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-dunav-ruse/hxATPUIK/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/cska-1948-sofia-maritsa-plovdiv/WS8XOlYQ/</t>
         </is>
       </c>
     </row>
@@ -1585,22 +1585,22 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>CSKA 1948 Sofia II</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" t="n">
-        <v>1.27</v>
+        <v>3.14</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -1608,15 +1608,15 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>1.49</v>
+        <v>3.17</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>22/07/2023 17:27</t>
+          <t>22/07/2023 17:28</t>
         </is>
       </c>
       <c r="N13" t="n">
-        <v>4.63</v>
+        <v>2.96</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1624,15 +1624,15 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>3.91</v>
+        <v>3.09</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>22/07/2023 17:27</t>
+          <t>22/07/2023 17:28</t>
         </is>
       </c>
       <c r="R13" t="n">
-        <v>6.8</v>
+        <v>2.04</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
@@ -1640,16 +1640,16 @@
         </is>
       </c>
       <c r="T13" t="n">
-        <v>5.61</v>
+        <v>2.14</v>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>22/07/2023 17:27</t>
+          <t>22/07/2023 17:28</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/cska-1948-sofia-maritsa-plovdiv/WS8XOlYQ/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-dunav-ruse/hxATPUIK/</t>
         </is>
       </c>
     </row>
@@ -1677,71 +1677,71 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>Litex Lovech</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>3.9</v>
+        <v>2.42</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>22/07/2023 16:45</t>
+          <t>21/07/2023 06:42</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>2.88</v>
+        <v>3.82</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>22/07/2023 18:18</t>
+          <t>22/07/2023 18:29</t>
         </is>
       </c>
       <c r="N14" t="n">
-        <v>3.59</v>
+        <v>2.69</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>22/07/2023 16:45</t>
+          <t>21/07/2023 06:42</t>
         </is>
       </c>
       <c r="P14" t="n">
-        <v>3.48</v>
+        <v>3</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>22/07/2023 18:18</t>
+          <t>22/07/2023 18:24</t>
         </is>
       </c>
       <c r="R14" t="n">
-        <v>1.75</v>
+        <v>2.78</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>22/07/2023 16:45</t>
+          <t>21/07/2023 06:42</t>
         </is>
       </c>
       <c r="T14" t="n">
-        <v>2.13</v>
+        <v>1.79</v>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>22/07/2023 18:18</t>
+          <t>22/07/2023 18:29</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-strumska-slava/r7Sx37B7/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/litex-lovech-dobrudzha/pC6LRjl8/</t>
         </is>
       </c>
     </row>
@@ -1769,71 +1769,71 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Litex Lovech</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>2.42</v>
+        <v>3.9</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>21/07/2023 06:42</t>
+          <t>22/07/2023 16:45</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>3.82</v>
+        <v>2.88</v>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>22/07/2023 18:29</t>
+          <t>22/07/2023 18:18</t>
         </is>
       </c>
       <c r="N15" t="n">
-        <v>2.69</v>
+        <v>3.59</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>21/07/2023 06:42</t>
+          <t>22/07/2023 16:45</t>
         </is>
       </c>
       <c r="P15" t="n">
-        <v>3</v>
+        <v>3.48</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>22/07/2023 18:24</t>
+          <t>22/07/2023 18:18</t>
         </is>
       </c>
       <c r="R15" t="n">
-        <v>2.78</v>
+        <v>1.75</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>21/07/2023 06:42</t>
+          <t>22/07/2023 16:45</t>
         </is>
       </c>
       <c r="T15" t="n">
-        <v>1.79</v>
+        <v>2.13</v>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>22/07/2023 18:29</t>
+          <t>22/07/2023 18:18</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/litex-lovech-dobrudzha/pC6LRjl8/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-strumska-slava/r7Sx37B7/</t>
         </is>
       </c>
     </row>
@@ -2229,71 +2229,71 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Litex Lovech</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>2.08</v>
+        <v>2.85</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>28/07/2023 05:42</t>
+          <t>29/07/2023 13:12</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>2.01</v>
+        <v>2.73</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>29/07/2023 17:02</t>
+          <t>29/07/2023 16:46</t>
         </is>
       </c>
       <c r="N20" t="n">
-        <v>2.82</v>
+        <v>2.97</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>28/07/2023 05:42</t>
+          <t>29/07/2023 13:12</t>
         </is>
       </c>
       <c r="P20" t="n">
-        <v>2.9</v>
+        <v>3.27</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>29/07/2023 17:02</t>
+          <t>29/07/2023 16:46</t>
         </is>
       </c>
       <c r="R20" t="n">
-        <v>3.21</v>
+        <v>2.36</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>28/07/2023 05:42</t>
+          <t>29/07/2023 13:12</t>
         </is>
       </c>
       <c r="T20" t="n">
-        <v>3.78</v>
+        <v>2.31</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>29/07/2023 17:02</t>
+          <t>29/07/2023 16:46</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-litex-lovech/OvPtXoQm/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-marek/McmCH6Q0/</t>
         </is>
       </c>
     </row>
@@ -2321,22 +2321,22 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>CSKA 1948 Sofia II</t>
+          <t>Litex Lovech</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J21" t="n">
-        <v>2.62</v>
+        <v>2.08</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -2344,15 +2344,15 @@
         </is>
       </c>
       <c r="L21" t="n">
-        <v>2.39</v>
+        <v>2.01</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>29/07/2023 16:28</t>
+          <t>29/07/2023 17:02</t>
         </is>
       </c>
       <c r="N21" t="n">
-        <v>2.84</v>
+        <v>2.82</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2360,15 +2360,15 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>3.18</v>
+        <v>2.9</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>29/07/2023 15:36</t>
+          <t>29/07/2023 17:02</t>
         </is>
       </c>
       <c r="R21" t="n">
-        <v>2.48</v>
+        <v>3.21</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
@@ -2376,16 +2376,16 @@
         </is>
       </c>
       <c r="T21" t="n">
-        <v>2.69</v>
+        <v>3.78</v>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>29/07/2023 16:28</t>
+          <t>29/07/2023 17:02</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-cska-1948-sofia/pWY6wlmK/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-litex-lovech/OvPtXoQm/</t>
         </is>
       </c>
     </row>
@@ -2413,22 +2413,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Ludogorets II</t>
+          <t>CSKA 1948 Sofia II</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J22" t="n">
-        <v>1.5</v>
+        <v>2.62</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -2436,15 +2436,15 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>1.5</v>
+        <v>2.39</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>29/07/2023 17:03</t>
+          <t>29/07/2023 16:28</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.63</v>
+        <v>2.84</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2452,15 +2452,15 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.82</v>
+        <v>3.18</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>29/07/2023 17:03</t>
+          <t>29/07/2023 15:36</t>
         </is>
       </c>
       <c r="R22" t="n">
-        <v>5.07</v>
+        <v>2.48</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
@@ -2468,16 +2468,16 @@
         </is>
       </c>
       <c r="T22" t="n">
-        <v>5.69</v>
+        <v>2.69</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>29/07/2023 17:03</t>
+          <t>29/07/2023 16:28</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-ludogorets/U3AwYRAs/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-cska-1948-sofia/pWY6wlmK/</t>
         </is>
       </c>
     </row>
@@ -2505,71 +2505,71 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="G23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Ludogorets II</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
         <v>0</v>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Marek</t>
-        </is>
-      </c>
-      <c r="I23" t="n">
-        <v>1</v>
-      </c>
       <c r="J23" t="n">
-        <v>2.85</v>
+        <v>1.5</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>29/07/2023 13:12</t>
+          <t>28/07/2023 05:42</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>2.73</v>
+        <v>1.5</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>29/07/2023 16:46</t>
+          <t>29/07/2023 17:03</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>2.97</v>
+        <v>3.63</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>29/07/2023 13:12</t>
+          <t>28/07/2023 05:42</t>
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3.27</v>
+        <v>3.82</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>29/07/2023 16:46</t>
+          <t>29/07/2023 17:03</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>2.36</v>
+        <v>5.07</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>29/07/2023 13:12</t>
+          <t>28/07/2023 05:42</t>
         </is>
       </c>
       <c r="T23" t="n">
-        <v>2.31</v>
+        <v>5.69</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>29/07/2023 16:46</t>
+          <t>29/07/2023 17:03</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-marek/McmCH6Q0/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-ludogorets/U3AwYRAs/</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Belasitsa</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -2605,14 +2605,14 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="n">
-        <v>1.5</v>
+        <v>1.92</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -2620,15 +2620,15 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>1.42</v>
+        <v>1.93</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>29/07/2023 18:03</t>
+          <t>29/07/2023 18:58</t>
         </is>
       </c>
       <c r="N24" t="n">
-        <v>3.96</v>
+        <v>3.07</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2636,15 +2636,15 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>4.09</v>
+        <v>3.69</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>29/07/2023 18:13</t>
+          <t>29/07/2023 18:58</t>
         </is>
       </c>
       <c r="R24" t="n">
-        <v>5.22</v>
+        <v>3.65</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2652,16 +2652,16 @@
         </is>
       </c>
       <c r="T24" t="n">
-        <v>6.42</v>
+        <v>3.16</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>29/07/2023 18:13</t>
+          <t>29/07/2023 18:58</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-chernomorets-balchik/2VNpW5uf/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/belasitsa-petrich-chernomorets-1919/vZsHGQu7/</t>
         </is>
       </c>
     </row>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Belasitsa</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -2697,14 +2697,14 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>1.92</v>
+        <v>1.5</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -2712,15 +2712,15 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>1.93</v>
+        <v>1.42</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>29/07/2023 18:58</t>
+          <t>29/07/2023 18:03</t>
         </is>
       </c>
       <c r="N25" t="n">
-        <v>3.07</v>
+        <v>3.96</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2728,15 +2728,15 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>3.69</v>
+        <v>4.09</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>29/07/2023 18:58</t>
+          <t>29/07/2023 18:13</t>
         </is>
       </c>
       <c r="R25" t="n">
-        <v>3.65</v>
+        <v>5.22</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
@@ -2744,16 +2744,16 @@
         </is>
       </c>
       <c r="T25" t="n">
-        <v>3.16</v>
+        <v>6.42</v>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>29/07/2023 18:58</t>
+          <t>29/07/2023 18:13</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/belasitsa-petrich-chernomorets-1919/vZsHGQu7/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-chernomorets-balchik/2VNpW5uf/</t>
         </is>
       </c>
     </row>
@@ -3241,22 +3241,22 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Yantra Gabrovo</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="I31" t="n">
         <v>1</v>
       </c>
       <c r="J31" t="n">
-        <v>2.09</v>
+        <v>1.55</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -3264,15 +3264,15 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>1.99</v>
+        <v>1.79</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>05/08/2023 16:45</t>
+          <t>05/08/2023 16:39</t>
         </is>
       </c>
       <c r="N31" t="n">
-        <v>2.89</v>
+        <v>3.5</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -3280,15 +3280,15 @@
         </is>
       </c>
       <c r="P31" t="n">
-        <v>3.01</v>
+        <v>3.24</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>05/08/2023 16:45</t>
+          <t>05/08/2023 16:39</t>
         </is>
       </c>
       <c r="R31" t="n">
-        <v>3.1</v>
+        <v>4.58</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
@@ -3296,16 +3296,16 @@
         </is>
       </c>
       <c r="T31" t="n">
-        <v>3.68</v>
+        <v>4.19</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>05/08/2023 16:45</t>
+          <t>05/08/2023 16:39</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-dunav-ruse/nJcljRWP/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/yantra-gabrovo-maritsa-plovdiv/4bpGoous/</t>
         </is>
       </c>
     </row>
@@ -3333,22 +3333,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Yantra Gabrovo</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="I32" t="n">
         <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>1.55</v>
+        <v>2.09</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -3356,15 +3356,15 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>1.79</v>
+        <v>1.99</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>05/08/2023 16:39</t>
+          <t>05/08/2023 16:45</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>3.5</v>
+        <v>2.89</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3372,15 +3372,15 @@
         </is>
       </c>
       <c r="P32" t="n">
-        <v>3.24</v>
+        <v>3.01</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>05/08/2023 16:39</t>
+          <t>05/08/2023 16:45</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>4.58</v>
+        <v>3.1</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
@@ -3388,16 +3388,16 @@
         </is>
       </c>
       <c r="T32" t="n">
-        <v>4.19</v>
+        <v>3.68</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>05/08/2023 16:39</t>
+          <t>05/08/2023 16:45</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/yantra-gabrovo-maritsa-plovdiv/4bpGoous/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-dunav-ruse/nJcljRWP/</t>
         </is>
       </c>
     </row>
@@ -3793,71 +3793,71 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Yantra Gabrovo</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="I37" t="n">
         <v>3</v>
       </c>
       <c r="J37" t="n">
-        <v>1.87</v>
+        <v>1.61</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>12/08/2023 05:12</t>
+          <t>13/08/2023 10:13</t>
         </is>
       </c>
       <c r="L37" t="n">
-        <v>1.65</v>
+        <v>1.68</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>13/08/2023 16:57</t>
+          <t>13/08/2023 16:52</t>
         </is>
       </c>
       <c r="N37" t="n">
-        <v>2.94</v>
+        <v>3.51</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>12/08/2023 05:12</t>
+          <t>13/08/2023 10:13</t>
         </is>
       </c>
       <c r="P37" t="n">
-        <v>3.27</v>
+        <v>3.93</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>13/08/2023 16:58</t>
+          <t>13/08/2023 16:52</t>
         </is>
       </c>
       <c r="R37" t="n">
-        <v>3.66</v>
+        <v>4.84</v>
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>12/08/2023 05:12</t>
+          <t>13/08/2023 10:13</t>
         </is>
       </c>
       <c r="T37" t="n">
-        <v>5.21</v>
+        <v>3.87</v>
       </c>
       <c r="U37" t="inlineStr">
         <is>
-          <t>13/08/2023 16:58</t>
+          <t>13/08/2023 16:52</t>
         </is>
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-yantra-gabrovo/SxVuts9I/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-chernomorets-1919/pEuysNgC/</t>
         </is>
       </c>
     </row>
@@ -3977,71 +3977,71 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Yantra Gabrovo</t>
         </is>
       </c>
       <c r="I39" t="n">
         <v>3</v>
       </c>
       <c r="J39" t="n">
-        <v>1.61</v>
+        <v>1.87</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>13/08/2023 10:13</t>
+          <t>12/08/2023 05:12</t>
         </is>
       </c>
       <c r="L39" t="n">
-        <v>1.68</v>
+        <v>1.65</v>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>13/08/2023 16:52</t>
+          <t>13/08/2023 16:57</t>
         </is>
       </c>
       <c r="N39" t="n">
-        <v>3.51</v>
+        <v>2.94</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>13/08/2023 10:13</t>
+          <t>12/08/2023 05:12</t>
         </is>
       </c>
       <c r="P39" t="n">
-        <v>3.93</v>
+        <v>3.27</v>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>13/08/2023 16:52</t>
+          <t>13/08/2023 16:58</t>
         </is>
       </c>
       <c r="R39" t="n">
-        <v>4.84</v>
+        <v>3.66</v>
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>13/08/2023 10:13</t>
+          <t>12/08/2023 05:12</t>
         </is>
       </c>
       <c r="T39" t="n">
-        <v>3.87</v>
+        <v>5.21</v>
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>13/08/2023 16:52</t>
+          <t>13/08/2023 16:58</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-chernomorets-1919/pEuysNgC/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-yantra-gabrovo/SxVuts9I/</t>
         </is>
       </c>
     </row>
@@ -7105,22 +7105,22 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="I73" t="n">
         <v>0</v>
       </c>
       <c r="J73" t="n">
-        <v>1.27</v>
+        <v>3.17</v>
       </c>
       <c r="K73" t="inlineStr">
         <is>
@@ -7128,15 +7128,15 @@
         </is>
       </c>
       <c r="L73" t="n">
-        <v>1.2</v>
+        <v>2.61</v>
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>17/09/2023 15:56</t>
+          <t>17/09/2023 15:49</t>
         </is>
       </c>
       <c r="N73" t="n">
-        <v>4.38</v>
+        <v>2.89</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -7144,15 +7144,15 @@
         </is>
       </c>
       <c r="P73" t="n">
-        <v>5.25</v>
+        <v>2.98</v>
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>17/09/2023 15:56</t>
+          <t>17/09/2023 15:49</t>
         </is>
       </c>
       <c r="R73" t="n">
-        <v>7.61</v>
+        <v>2.06</v>
       </c>
       <c r="S73" t="inlineStr">
         <is>
@@ -7160,16 +7160,16 @@
         </is>
       </c>
       <c r="T73" t="n">
-        <v>13.6</v>
+        <v>2.6</v>
       </c>
       <c r="U73" t="inlineStr">
         <is>
-          <t>17/09/2023 15:56</t>
+          <t>17/09/2023 15:49</t>
         </is>
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-bdin-vidin/r767L9SR/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-svoge/htdsF75e/</t>
         </is>
       </c>
     </row>
@@ -7197,22 +7197,22 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Spartak Varna</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="I74" t="n">
         <v>1</v>
       </c>
       <c r="J74" t="n">
-        <v>2.56</v>
+        <v>1.75</v>
       </c>
       <c r="K74" t="inlineStr">
         <is>
@@ -7220,15 +7220,15 @@
         </is>
       </c>
       <c r="L74" t="n">
-        <v>3.02</v>
+        <v>1.75</v>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>17/09/2023 15:46</t>
+          <t>17/09/2023 15:09</t>
         </is>
       </c>
       <c r="N74" t="n">
-        <v>2.73</v>
+        <v>3.17</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -7236,15 +7236,15 @@
         </is>
       </c>
       <c r="P74" t="n">
-        <v>2.66</v>
+        <v>3.18</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>17/09/2023 15:46</t>
+          <t>17/09/2023 15:23</t>
         </is>
       </c>
       <c r="R74" t="n">
-        <v>2.63</v>
+        <v>3.84</v>
       </c>
       <c r="S74" t="inlineStr">
         <is>
@@ -7252,16 +7252,16 @@
         </is>
       </c>
       <c r="T74" t="n">
-        <v>2.52</v>
+        <v>4.58</v>
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>17/09/2023 15:46</t>
+          <t>17/09/2023 15:08</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-spartak-varna/MiIbNVcF/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-chernomorets-1919/KScZGTzq/</t>
         </is>
       </c>
     </row>
@@ -7289,22 +7289,22 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>Ludogorets II</t>
         </is>
       </c>
       <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Spartak Pleven</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
         <v>2</v>
       </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>Svoge</t>
-        </is>
-      </c>
-      <c r="I75" t="n">
-        <v>0</v>
-      </c>
       <c r="J75" t="n">
-        <v>3.17</v>
+        <v>1.55</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
@@ -7312,15 +7312,15 @@
         </is>
       </c>
       <c r="L75" t="n">
-        <v>2.61</v>
+        <v>1.61</v>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>17/09/2023 15:49</t>
+          <t>17/09/2023 15:57</t>
         </is>
       </c>
       <c r="N75" t="n">
-        <v>2.89</v>
+        <v>3.54</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -7328,15 +7328,15 @@
         </is>
       </c>
       <c r="P75" t="n">
-        <v>2.98</v>
+        <v>3.49</v>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>17/09/2023 15:49</t>
+          <t>17/09/2023 15:57</t>
         </is>
       </c>
       <c r="R75" t="n">
-        <v>2.06</v>
+        <v>4.49</v>
       </c>
       <c r="S75" t="inlineStr">
         <is>
@@ -7344,16 +7344,16 @@
         </is>
       </c>
       <c r="T75" t="n">
-        <v>2.6</v>
+        <v>4.09</v>
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>17/09/2023 15:49</t>
+          <t>17/09/2023 15:57</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-svoge/htdsF75e/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-spartak-pleven/bgRsDoz8/</t>
         </is>
       </c>
     </row>
@@ -7381,22 +7381,22 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="G76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Spartak Varna</t>
         </is>
       </c>
       <c r="I76" t="n">
         <v>1</v>
       </c>
       <c r="J76" t="n">
-        <v>1.75</v>
+        <v>2.56</v>
       </c>
       <c r="K76" t="inlineStr">
         <is>
@@ -7404,15 +7404,15 @@
         </is>
       </c>
       <c r="L76" t="n">
-        <v>1.75</v>
+        <v>3.02</v>
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>17/09/2023 15:09</t>
+          <t>17/09/2023 15:46</t>
         </is>
       </c>
       <c r="N76" t="n">
-        <v>3.17</v>
+        <v>2.73</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -7420,15 +7420,15 @@
         </is>
       </c>
       <c r="P76" t="n">
-        <v>3.18</v>
+        <v>2.66</v>
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>17/09/2023 15:23</t>
+          <t>17/09/2023 15:46</t>
         </is>
       </c>
       <c r="R76" t="n">
-        <v>3.84</v>
+        <v>2.63</v>
       </c>
       <c r="S76" t="inlineStr">
         <is>
@@ -7436,16 +7436,16 @@
         </is>
       </c>
       <c r="T76" t="n">
-        <v>4.58</v>
+        <v>2.52</v>
       </c>
       <c r="U76" t="inlineStr">
         <is>
-          <t>17/09/2023 15:08</t>
+          <t>17/09/2023 15:46</t>
         </is>
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-chernomorets-1919/KScZGTzq/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-spartak-varna/MiIbNVcF/</t>
         </is>
       </c>
     </row>
@@ -7473,22 +7473,22 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Ludogorets II</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="G77" t="n">
+        <v>1</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Bdin Vidin</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
         <v>0</v>
       </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>Spartak Pleven</t>
-        </is>
-      </c>
-      <c r="I77" t="n">
-        <v>2</v>
-      </c>
       <c r="J77" t="n">
-        <v>1.55</v>
+        <v>1.27</v>
       </c>
       <c r="K77" t="inlineStr">
         <is>
@@ -7496,15 +7496,15 @@
         </is>
       </c>
       <c r="L77" t="n">
-        <v>1.61</v>
+        <v>1.2</v>
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>17/09/2023 15:57</t>
+          <t>17/09/2023 15:56</t>
         </is>
       </c>
       <c r="N77" t="n">
-        <v>3.54</v>
+        <v>4.38</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -7512,15 +7512,15 @@
         </is>
       </c>
       <c r="P77" t="n">
-        <v>3.49</v>
+        <v>5.25</v>
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>17/09/2023 15:57</t>
+          <t>17/09/2023 15:56</t>
         </is>
       </c>
       <c r="R77" t="n">
-        <v>4.49</v>
+        <v>7.61</v>
       </c>
       <c r="S77" t="inlineStr">
         <is>
@@ -7528,16 +7528,16 @@
         </is>
       </c>
       <c r="T77" t="n">
-        <v>4.09</v>
+        <v>13.6</v>
       </c>
       <c r="U77" t="inlineStr">
         <is>
-          <t>17/09/2023 15:57</t>
+          <t>17/09/2023 15:56</t>
         </is>
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-spartak-pleven/bgRsDoz8/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-bdin-vidin/r767L9SR/</t>
         </is>
       </c>
     </row>
@@ -7933,22 +7933,22 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="I82" t="n">
         <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>1.55</v>
+        <v>2.38</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
@@ -7956,15 +7956,15 @@
         </is>
       </c>
       <c r="L82" t="n">
-        <v>1.95</v>
+        <v>2.33</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>22/09/2023 15:56</t>
+          <t>22/09/2023 15:59</t>
         </is>
       </c>
       <c r="N82" t="n">
-        <v>3.45</v>
+        <v>2.93</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -7972,15 +7972,15 @@
         </is>
       </c>
       <c r="P82" t="n">
-        <v>3.51</v>
+        <v>2.97</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>22/09/2023 15:56</t>
+          <t>22/09/2023 15:59</t>
         </is>
       </c>
       <c r="R82" t="n">
-        <v>4.66</v>
+        <v>2.6</v>
       </c>
       <c r="S82" t="inlineStr">
         <is>
@@ -7988,16 +7988,16 @@
         </is>
       </c>
       <c r="T82" t="n">
-        <v>3.24</v>
+        <v>2.96</v>
       </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>22/09/2023 15:56</t>
+          <t>22/09/2023 15:59</t>
         </is>
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-spartak-pleven/CdFPyVC8/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-dunav-ruse/6JjLQ447/</t>
         </is>
       </c>
     </row>
@@ -8025,22 +8025,22 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="I83" t="n">
         <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>2.38</v>
+        <v>1.55</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -8048,15 +8048,15 @@
         </is>
       </c>
       <c r="L83" t="n">
-        <v>2.33</v>
+        <v>1.95</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>22/09/2023 15:59</t>
+          <t>22/09/2023 15:56</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>2.93</v>
+        <v>3.45</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -8064,15 +8064,15 @@
         </is>
       </c>
       <c r="P83" t="n">
-        <v>2.97</v>
+        <v>3.51</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>22/09/2023 15:59</t>
+          <t>22/09/2023 15:56</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>2.6</v>
+        <v>4.66</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
@@ -8080,16 +8080,16 @@
         </is>
       </c>
       <c r="T83" t="n">
-        <v>2.96</v>
+        <v>3.24</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>22/09/2023 15:59</t>
+          <t>22/09/2023 15:56</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-dunav-ruse/6JjLQ447/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-spartak-pleven/CdFPyVC8/</t>
         </is>
       </c>
     </row>
@@ -9221,22 +9221,22 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Septemvri Sofia</t>
         </is>
       </c>
       <c r="G96" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Spartak Varna</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="I96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J96" t="n">
-        <v>2.15</v>
+        <v>1.4</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
@@ -9244,7 +9244,7 @@
         </is>
       </c>
       <c r="L96" t="n">
-        <v>1.93</v>
+        <v>1.3</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
@@ -9252,7 +9252,7 @@
         </is>
       </c>
       <c r="N96" t="n">
-        <v>2.77</v>
+        <v>4.04</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -9260,15 +9260,15 @@
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.23</v>
+        <v>4.83</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
-          <t>28/09/2023 15:59</t>
+          <t>28/09/2023 15:58</t>
         </is>
       </c>
       <c r="R96" t="n">
-        <v>3.11</v>
+        <v>5.31</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
@@ -9276,16 +9276,16 @@
         </is>
       </c>
       <c r="T96" t="n">
-        <v>3.57</v>
+        <v>7.8</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>28/09/2023 15:59</t>
+          <t>28/09/2023 15:58</t>
         </is>
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-spartak-varna/0KrZGlht/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/septemvri-sofia-maritsa-plovdiv/OfL5YGND/</t>
         </is>
       </c>
     </row>
@@ -9405,22 +9405,22 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Septemvri Sofia</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="G98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Spartak Varna</t>
         </is>
       </c>
       <c r="I98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>1.4</v>
+        <v>2.15</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -9428,7 +9428,7 @@
         </is>
       </c>
       <c r="L98" t="n">
-        <v>1.3</v>
+        <v>1.93</v>
       </c>
       <c r="M98" t="inlineStr">
         <is>
@@ -9436,7 +9436,7 @@
         </is>
       </c>
       <c r="N98" t="n">
-        <v>4.04</v>
+        <v>2.77</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -9444,15 +9444,15 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>4.83</v>
+        <v>3.23</v>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
-          <t>28/09/2023 15:58</t>
+          <t>28/09/2023 15:59</t>
         </is>
       </c>
       <c r="R98" t="n">
-        <v>5.31</v>
+        <v>3.11</v>
       </c>
       <c r="S98" t="inlineStr">
         <is>
@@ -9460,16 +9460,16 @@
         </is>
       </c>
       <c r="T98" t="n">
-        <v>7.8</v>
+        <v>3.57</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
-          <t>28/09/2023 15:58</t>
+          <t>28/09/2023 15:59</t>
         </is>
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/septemvri-sofia-maritsa-plovdiv/OfL5YGND/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-spartak-varna/0KrZGlht/</t>
         </is>
       </c>
     </row>
@@ -9589,7 +9589,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="G100" t="n">
@@ -9597,14 +9597,14 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>CSKA 1948 Sofia II</t>
         </is>
       </c>
       <c r="I100" t="n">
         <v>0</v>
       </c>
       <c r="J100" t="n">
-        <v>2.05</v>
+        <v>2.87</v>
       </c>
       <c r="K100" t="inlineStr">
         <is>
@@ -9612,15 +9612,15 @@
         </is>
       </c>
       <c r="L100" t="n">
-        <v>1.82</v>
+        <v>2.17</v>
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>01/10/2023 14:52</t>
+          <t>01/10/2023 14:51</t>
         </is>
       </c>
       <c r="N100" t="n">
-        <v>2.84</v>
+        <v>2.78</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -9632,11 +9632,11 @@
       </c>
       <c r="Q100" t="inlineStr">
         <is>
-          <t>01/10/2023 14:52</t>
+          <t>01/10/2023 14:40</t>
         </is>
       </c>
       <c r="R100" t="n">
-        <v>3.25</v>
+        <v>2.29</v>
       </c>
       <c r="S100" t="inlineStr">
         <is>
@@ -9644,16 +9644,16 @@
         </is>
       </c>
       <c r="T100" t="n">
-        <v>4.16</v>
+        <v>3.04</v>
       </c>
       <c r="U100" t="inlineStr">
         <is>
-          <t>01/10/2023 14:52</t>
+          <t>01/10/2023 14:51</t>
         </is>
       </c>
       <c r="V100" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-chernomorets-balchik/xp2uON5N/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-cska-1948-sofia/OMePR56b/</t>
         </is>
       </c>
     </row>
@@ -9681,7 +9681,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="G101" t="n">
@@ -9689,14 +9689,14 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>CSKA 1948 Sofia II</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="I101" t="n">
         <v>0</v>
       </c>
       <c r="J101" t="n">
-        <v>2.87</v>
+        <v>2.05</v>
       </c>
       <c r="K101" t="inlineStr">
         <is>
@@ -9704,15 +9704,15 @@
         </is>
       </c>
       <c r="L101" t="n">
-        <v>2.17</v>
+        <v>1.82</v>
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>01/10/2023 14:51</t>
+          <t>01/10/2023 14:52</t>
         </is>
       </c>
       <c r="N101" t="n">
-        <v>2.78</v>
+        <v>2.84</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -9724,11 +9724,11 @@
       </c>
       <c r="Q101" t="inlineStr">
         <is>
-          <t>01/10/2023 14:40</t>
+          <t>01/10/2023 14:52</t>
         </is>
       </c>
       <c r="R101" t="n">
-        <v>2.29</v>
+        <v>3.25</v>
       </c>
       <c r="S101" t="inlineStr">
         <is>
@@ -9736,16 +9736,16 @@
         </is>
       </c>
       <c r="T101" t="n">
-        <v>3.04</v>
+        <v>4.16</v>
       </c>
       <c r="U101" t="inlineStr">
         <is>
-          <t>01/10/2023 14:51</t>
+          <t>01/10/2023 14:52</t>
         </is>
       </c>
       <c r="V101" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-cska-1948-sofia/OMePR56b/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-chernomorets-balchik/xp2uON5N/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,14 +9781,14 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Septemvri Sofia</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J102" t="n">
-        <v>2.49</v>
+        <v>1.76</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
@@ -9796,15 +9796,15 @@
         </is>
       </c>
       <c r="L102" t="n">
-        <v>3.42</v>
+        <v>1.88</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>02/10/2023 14:46</t>
+          <t>02/10/2023 14:57</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>2.82</v>
+        <v>3.15</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
@@ -9812,15 +9812,15 @@
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.04</v>
+        <v>3.33</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>02/10/2023 14:46</t>
+          <t>02/10/2023 14:57</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>2.56</v>
+        <v>3.82</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
@@ -9828,16 +9828,16 @@
         </is>
       </c>
       <c r="T102" t="n">
-        <v>2.07</v>
+        <v>3.65</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>02/10/2023 14:08</t>
+          <t>02/10/2023 14:57</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-septemvri-sofia/Ozybt5Li/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-spartak-pleven/IqeTQPL4/</t>
         </is>
       </c>
     </row>
@@ -9957,7 +9957,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="G104" t="n">
@@ -9965,14 +9965,14 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Septemvri Sofia</t>
         </is>
       </c>
       <c r="I104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J104" t="n">
-        <v>1.76</v>
+        <v>2.49</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
@@ -9980,15 +9980,15 @@
         </is>
       </c>
       <c r="L104" t="n">
-        <v>1.88</v>
+        <v>3.42</v>
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>02/10/2023 14:57</t>
+          <t>02/10/2023 14:46</t>
         </is>
       </c>
       <c r="N104" t="n">
-        <v>3.15</v>
+        <v>2.82</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
@@ -9996,15 +9996,15 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>3.33</v>
+        <v>3.04</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>02/10/2023 14:57</t>
+          <t>02/10/2023 14:46</t>
         </is>
       </c>
       <c r="R104" t="n">
-        <v>3.82</v>
+        <v>2.56</v>
       </c>
       <c r="S104" t="inlineStr">
         <is>
@@ -10012,16 +10012,16 @@
         </is>
       </c>
       <c r="T104" t="n">
-        <v>3.65</v>
+        <v>2.07</v>
       </c>
       <c r="U104" t="inlineStr">
         <is>
-          <t>02/10/2023 14:57</t>
+          <t>02/10/2023 14:08</t>
         </is>
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-spartak-pleven/IqeTQPL4/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dunav-ruse-septemvri-sofia/Ozybt5Li/</t>
         </is>
       </c>
     </row>
@@ -10417,22 +10417,22 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Septemvri Sofia</t>
         </is>
       </c>
       <c r="G109" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>Dunav Ruse</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="I109" t="n">
         <v>0</v>
       </c>
       <c r="J109" t="n">
-        <v>1.65</v>
+        <v>1.53</v>
       </c>
       <c r="K109" t="inlineStr">
         <is>
@@ -10440,15 +10440,15 @@
         </is>
       </c>
       <c r="L109" t="n">
-        <v>1.48</v>
+        <v>1.4</v>
       </c>
       <c r="M109" t="inlineStr">
         <is>
-          <t>07/10/2023 14:51</t>
+          <t>07/10/2023 14:46</t>
         </is>
       </c>
       <c r="N109" t="n">
-        <v>3.13</v>
+        <v>3.51</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -10456,15 +10456,15 @@
         </is>
       </c>
       <c r="P109" t="n">
-        <v>3.64</v>
+        <v>4.03</v>
       </c>
       <c r="Q109" t="inlineStr">
         <is>
-          <t>07/10/2023 14:51</t>
+          <t>07/10/2023 14:46</t>
         </is>
       </c>
       <c r="R109" t="n">
-        <v>4.65</v>
+        <v>4.72</v>
       </c>
       <c r="S109" t="inlineStr">
         <is>
@@ -10472,16 +10472,16 @@
         </is>
       </c>
       <c r="T109" t="n">
-        <v>6.37</v>
+        <v>6.99</v>
       </c>
       <c r="U109" t="inlineStr">
         <is>
-          <t>07/10/2023 14:51</t>
+          <t>07/10/2023 14:46</t>
         </is>
       </c>
       <c r="V109" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-dunav-ruse/dlZ5vqj4/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/septemvri-sofia-marek/Icz2uPzb/</t>
         </is>
       </c>
     </row>
@@ -10601,22 +10601,22 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Septemvri Sofia</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="G111" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="I111" t="n">
         <v>0</v>
       </c>
       <c r="J111" t="n">
-        <v>1.53</v>
+        <v>1.65</v>
       </c>
       <c r="K111" t="inlineStr">
         <is>
@@ -10624,15 +10624,15 @@
         </is>
       </c>
       <c r="L111" t="n">
-        <v>1.4</v>
+        <v>1.48</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>07/10/2023 14:46</t>
+          <t>07/10/2023 14:51</t>
         </is>
       </c>
       <c r="N111" t="n">
-        <v>3.51</v>
+        <v>3.13</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -10640,15 +10640,15 @@
         </is>
       </c>
       <c r="P111" t="n">
-        <v>4.03</v>
+        <v>3.64</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>07/10/2023 14:46</t>
+          <t>07/10/2023 14:51</t>
         </is>
       </c>
       <c r="R111" t="n">
-        <v>4.72</v>
+        <v>4.65</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
@@ -10656,16 +10656,16 @@
         </is>
       </c>
       <c r="T111" t="n">
-        <v>6.99</v>
+        <v>6.37</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>07/10/2023 14:46</t>
+          <t>07/10/2023 14:51</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/septemvri-sofia-marek/Icz2uPzb/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-dunav-ruse/dlZ5vqj4/</t>
         </is>
       </c>
     </row>
@@ -11245,22 +11245,22 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="G118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>Ludogorets II</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="I118" t="n">
         <v>2</v>
       </c>
       <c r="J118" t="n">
-        <v>2.75</v>
+        <v>2.26</v>
       </c>
       <c r="K118" t="inlineStr">
         <is>
@@ -11268,15 +11268,15 @@
         </is>
       </c>
       <c r="L118" t="n">
-        <v>2.71</v>
+        <v>2.44</v>
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 14:48</t>
         </is>
       </c>
       <c r="N118" t="n">
-        <v>2.81</v>
+        <v>2.88</v>
       </c>
       <c r="O118" t="inlineStr">
         <is>
@@ -11284,15 +11284,15 @@
         </is>
       </c>
       <c r="P118" t="n">
-        <v>2.85</v>
+        <v>2.83</v>
       </c>
       <c r="Q118" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 14:48</t>
         </is>
       </c>
       <c r="R118" t="n">
-        <v>2.34</v>
+        <v>2.8</v>
       </c>
       <c r="S118" t="inlineStr">
         <is>
@@ -11300,16 +11300,16 @@
         </is>
       </c>
       <c r="T118" t="n">
-        <v>2.6</v>
+        <v>2.93</v>
       </c>
       <c r="U118" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 14:48</t>
         </is>
       </c>
       <c r="V118" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-ludogorets/OGEpjtkG/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-montana/MifLqvSq/</t>
         </is>
       </c>
     </row>
@@ -11337,22 +11337,22 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="G119" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="I119" t="n">
         <v>0</v>
       </c>
       <c r="J119" t="n">
-        <v>1.88</v>
+        <v>1.89</v>
       </c>
       <c r="K119" t="inlineStr">
         <is>
@@ -11360,15 +11360,15 @@
         </is>
       </c>
       <c r="L119" t="n">
-        <v>1.59</v>
+        <v>1.81</v>
       </c>
       <c r="M119" t="inlineStr">
         <is>
-          <t>21/10/2023 14:51</t>
+          <t>21/10/2023 14:54</t>
         </is>
       </c>
       <c r="N119" t="n">
-        <v>3.03</v>
+        <v>2.94</v>
       </c>
       <c r="O119" t="inlineStr">
         <is>
@@ -11376,15 +11376,15 @@
         </is>
       </c>
       <c r="P119" t="n">
-        <v>3.42</v>
+        <v>3.18</v>
       </c>
       <c r="Q119" t="inlineStr">
         <is>
-          <t>21/10/2023 14:51</t>
+          <t>21/10/2023 14:54</t>
         </is>
       </c>
       <c r="R119" t="n">
-        <v>3.48</v>
+        <v>3.71</v>
       </c>
       <c r="S119" t="inlineStr">
         <is>
@@ -11392,16 +11392,16 @@
         </is>
       </c>
       <c r="T119" t="n">
-        <v>5.4</v>
+        <v>4.22</v>
       </c>
       <c r="U119" t="inlineStr">
         <is>
-          <t>21/10/2023 14:51</t>
+          <t>21/10/2023 14:54</t>
         </is>
       </c>
       <c r="V119" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-1919-spartak-pleven/UgFtiMZ9/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-svoge/zeMXhr5c/</t>
         </is>
       </c>
     </row>
@@ -11429,22 +11429,22 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="G120" t="n">
+        <v>0</v>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Ludogorets II</t>
+        </is>
+      </c>
+      <c r="I120" t="n">
         <v>2</v>
       </c>
-      <c r="H120" t="inlineStr">
-        <is>
-          <t>Svoge</t>
-        </is>
-      </c>
-      <c r="I120" t="n">
-        <v>0</v>
-      </c>
       <c r="J120" t="n">
-        <v>1.89</v>
+        <v>2.75</v>
       </c>
       <c r="K120" t="inlineStr">
         <is>
@@ -11452,15 +11452,15 @@
         </is>
       </c>
       <c r="L120" t="n">
-        <v>1.81</v>
+        <v>2.71</v>
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>21/10/2023 14:54</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="N120" t="n">
-        <v>2.94</v>
+        <v>2.81</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -11468,15 +11468,15 @@
         </is>
       </c>
       <c r="P120" t="n">
-        <v>3.18</v>
+        <v>2.85</v>
       </c>
       <c r="Q120" t="inlineStr">
         <is>
-          <t>21/10/2023 14:54</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="R120" t="n">
-        <v>3.71</v>
+        <v>2.34</v>
       </c>
       <c r="S120" t="inlineStr">
         <is>
@@ -11484,16 +11484,16 @@
         </is>
       </c>
       <c r="T120" t="n">
-        <v>4.22</v>
+        <v>2.6</v>
       </c>
       <c r="U120" t="inlineStr">
         <is>
-          <t>21/10/2023 14:54</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-svoge/zeMXhr5c/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/bdin-vidin-ludogorets/OGEpjtkG/</t>
         </is>
       </c>
     </row>
@@ -11521,22 +11521,22 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="G121" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="I121" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J121" t="n">
-        <v>2.26</v>
+        <v>1.88</v>
       </c>
       <c r="K121" t="inlineStr">
         <is>
@@ -11544,15 +11544,15 @@
         </is>
       </c>
       <c r="L121" t="n">
-        <v>2.44</v>
+        <v>1.59</v>
       </c>
       <c r="M121" t="inlineStr">
         <is>
-          <t>21/10/2023 14:48</t>
+          <t>21/10/2023 14:51</t>
         </is>
       </c>
       <c r="N121" t="n">
-        <v>2.88</v>
+        <v>3.03</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -11560,15 +11560,15 @@
         </is>
       </c>
       <c r="P121" t="n">
-        <v>2.83</v>
+        <v>3.42</v>
       </c>
       <c r="Q121" t="inlineStr">
         <is>
-          <t>21/10/2023 14:48</t>
+          <t>21/10/2023 14:51</t>
         </is>
       </c>
       <c r="R121" t="n">
-        <v>2.8</v>
+        <v>3.48</v>
       </c>
       <c r="S121" t="inlineStr">
         <is>
@@ -11576,16 +11576,16 @@
         </is>
       </c>
       <c r="T121" t="n">
-        <v>2.93</v>
+        <v>5.4</v>
       </c>
       <c r="U121" t="inlineStr">
         <is>
-          <t>21/10/2023 14:48</t>
+          <t>21/10/2023 14:51</t>
         </is>
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-montana/MifLqvSq/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-1919-spartak-pleven/UgFtiMZ9/</t>
         </is>
       </c>
     </row>
@@ -11981,22 +11981,22 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="G126" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="I126" t="n">
         <v>0</v>
       </c>
       <c r="J126" t="n">
-        <v>2.39</v>
+        <v>1.66</v>
       </c>
       <c r="K126" t="inlineStr">
         <is>
@@ -12004,48 +12004,48 @@
         </is>
       </c>
       <c r="L126" t="n">
-        <v>2.07</v>
+        <v>1.62</v>
       </c>
       <c r="M126" t="inlineStr">
         <is>
+          <t>27/10/2023 14:53</t>
+        </is>
+      </c>
+      <c r="N126" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>26/10/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P126" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>27/10/2023 14:53</t>
+        </is>
+      </c>
+      <c r="R126" t="n">
+        <v>4.24</v>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>26/10/2023 03:12</t>
+        </is>
+      </c>
+      <c r="T126" t="n">
+        <v>5.62</v>
+      </c>
+      <c r="U126" t="inlineStr">
+        <is>
           <t>27/10/2023 14:51</t>
         </is>
       </c>
-      <c r="N126" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="O126" t="inlineStr">
-        <is>
-          <t>26/10/2023 03:12</t>
-        </is>
-      </c>
-      <c r="P126" t="n">
-        <v>3.23</v>
-      </c>
-      <c r="Q126" t="inlineStr">
-        <is>
-          <t>27/10/2023 14:51</t>
-        </is>
-      </c>
-      <c r="R126" t="n">
-        <v>2.59</v>
-      </c>
-      <c r="S126" t="inlineStr">
-        <is>
-          <t>26/10/2023 03:12</t>
-        </is>
-      </c>
-      <c r="T126" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="U126" t="inlineStr">
-        <is>
-          <t>27/10/2023 14:51</t>
-        </is>
-      </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-maritsa-plovdiv/rulN3aJF/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-bdin-vidin/W25apBIf/</t>
         </is>
       </c>
     </row>
@@ -12073,22 +12073,22 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>CSKA 1948 Sofia II</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="G127" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Yantra Gabrovo</t>
         </is>
       </c>
       <c r="I127" t="n">
         <v>0</v>
       </c>
       <c r="J127" t="n">
-        <v>1.46</v>
+        <v>2.52</v>
       </c>
       <c r="K127" t="inlineStr">
         <is>
@@ -12096,15 +12096,15 @@
         </is>
       </c>
       <c r="L127" t="n">
-        <v>1.51</v>
+        <v>3.05</v>
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>27/10/2023 14:53</t>
+          <t>27/10/2023 14:49</t>
         </is>
       </c>
       <c r="N127" t="n">
-        <v>3.67</v>
+        <v>2.7</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -12112,15 +12112,15 @@
         </is>
       </c>
       <c r="P127" t="n">
-        <v>3.64</v>
+        <v>2.51</v>
       </c>
       <c r="Q127" t="inlineStr">
         <is>
-          <t>27/10/2023 14:53</t>
+          <t>27/10/2023 14:46</t>
         </is>
       </c>
       <c r="R127" t="n">
-        <v>5.19</v>
+        <v>2.64</v>
       </c>
       <c r="S127" t="inlineStr">
         <is>
@@ -12128,16 +12128,16 @@
         </is>
       </c>
       <c r="T127" t="n">
-        <v>5.9</v>
+        <v>2.64</v>
       </c>
       <c r="U127" t="inlineStr">
         <is>
-          <t>27/10/2023 14:53</t>
+          <t>27/10/2023 14:49</t>
         </is>
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/cska-1948-sofia-chernomorets-1919/Ag43qVX0/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-yantra-gabrovo/SUb8rkm7/</t>
         </is>
       </c>
     </row>
@@ -12165,22 +12165,22 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Dobrudzha</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="G128" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Septemvri Sofia</t>
         </is>
       </c>
       <c r="I128" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J128" t="n">
-        <v>1.54</v>
+        <v>3.35</v>
       </c>
       <c r="K128" t="inlineStr">
         <is>
@@ -12188,15 +12188,15 @@
         </is>
       </c>
       <c r="L128" t="n">
-        <v>1.42</v>
+        <v>3.78</v>
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>27/10/2023 14:53</t>
+          <t>27/10/2023 14:50</t>
         </is>
       </c>
       <c r="N128" t="n">
-        <v>3.39</v>
+        <v>2.93</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -12204,15 +12204,15 @@
         </is>
       </c>
       <c r="P128" t="n">
-        <v>3.83</v>
+        <v>3.4</v>
       </c>
       <c r="Q128" t="inlineStr">
         <is>
-          <t>27/10/2023 14:53</t>
+          <t>27/10/2023 14:50</t>
         </is>
       </c>
       <c r="R128" t="n">
-        <v>4.81</v>
+        <v>1.95</v>
       </c>
       <c r="S128" t="inlineStr">
         <is>
@@ -12220,16 +12220,16 @@
         </is>
       </c>
       <c r="T128" t="n">
-        <v>7.25</v>
+        <v>1.83</v>
       </c>
       <c r="U128" t="inlineStr">
         <is>
-          <t>27/10/2023 14:53</t>
+          <t>27/10/2023 14:50</t>
         </is>
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-marek/WMyC61Zd/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-septemvri-sofia/ADzG5Ll3/</t>
         </is>
       </c>
     </row>
@@ -12257,22 +12257,22 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Ludogorets II</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="G129" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Belasitsa</t>
+          <t>Dunav Ruse</t>
         </is>
       </c>
       <c r="I129" t="n">
         <v>1</v>
       </c>
       <c r="J129" t="n">
-        <v>1.68</v>
+        <v>2</v>
       </c>
       <c r="K129" t="inlineStr">
         <is>
@@ -12280,15 +12280,15 @@
         </is>
       </c>
       <c r="L129" t="n">
-        <v>1.6</v>
+        <v>1.85</v>
       </c>
       <c r="M129" t="inlineStr">
         <is>
-          <t>27/10/2023 13:03</t>
+          <t>27/10/2023 14:48</t>
         </is>
       </c>
       <c r="N129" t="n">
-        <v>3.24</v>
+        <v>2.86</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -12296,15 +12296,15 @@
         </is>
       </c>
       <c r="P129" t="n">
-        <v>3.51</v>
+        <v>2.88</v>
       </c>
       <c r="Q129" t="inlineStr">
         <is>
-          <t>27/10/2023 13:41</t>
+          <t>27/10/2023 14:48</t>
         </is>
       </c>
       <c r="R129" t="n">
-        <v>4.05</v>
+        <v>3.34</v>
       </c>
       <c r="S129" t="inlineStr">
         <is>
@@ -12312,16 +12312,16 @@
         </is>
       </c>
       <c r="T129" t="n">
-        <v>5.13</v>
+        <v>4.6</v>
       </c>
       <c r="U129" t="inlineStr">
         <is>
-          <t>27/10/2023 13:03</t>
+          <t>27/10/2023 14:48</t>
         </is>
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-belasitsa-petrich/xt6eoi3l/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-dunav-ruse/4lkJ4u49/</t>
         </is>
       </c>
     </row>
@@ -12349,22 +12349,22 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="G130" t="n">
+        <v>1</v>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>Maritsa Plovdiv</t>
+        </is>
+      </c>
+      <c r="I130" t="n">
         <v>0</v>
       </c>
-      <c r="H130" t="inlineStr">
-        <is>
-          <t>Dunav Ruse</t>
-        </is>
-      </c>
-      <c r="I130" t="n">
-        <v>1</v>
-      </c>
       <c r="J130" t="n">
-        <v>2</v>
+        <v>2.39</v>
       </c>
       <c r="K130" t="inlineStr">
         <is>
@@ -12372,15 +12372,15 @@
         </is>
       </c>
       <c r="L130" t="n">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>27/10/2023 14:48</t>
+          <t>27/10/2023 14:51</t>
         </is>
       </c>
       <c r="N130" t="n">
-        <v>2.86</v>
+        <v>2.92</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -12388,15 +12388,15 @@
         </is>
       </c>
       <c r="P130" t="n">
-        <v>2.88</v>
+        <v>3.23</v>
       </c>
       <c r="Q130" t="inlineStr">
         <is>
-          <t>27/10/2023 14:48</t>
+          <t>27/10/2023 14:51</t>
         </is>
       </c>
       <c r="R130" t="n">
-        <v>3.34</v>
+        <v>2.59</v>
       </c>
       <c r="S130" t="inlineStr">
         <is>
@@ -12404,16 +12404,16 @@
         </is>
       </c>
       <c r="T130" t="n">
-        <v>4.6</v>
+        <v>3.2</v>
       </c>
       <c r="U130" t="inlineStr">
         <is>
-          <t>27/10/2023 14:48</t>
+          <t>27/10/2023 14:51</t>
         </is>
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/montana-dunav-ruse/4lkJ4u49/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-maritsa-plovdiv/rulN3aJF/</t>
         </is>
       </c>
     </row>
@@ -12441,22 +12441,22 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Dobrudzha</t>
         </is>
       </c>
       <c r="G131" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>Bdin Vidin</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="I131" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J131" t="n">
-        <v>1.66</v>
+        <v>1.54</v>
       </c>
       <c r="K131" t="inlineStr">
         <is>
@@ -12464,7 +12464,7 @@
         </is>
       </c>
       <c r="L131" t="n">
-        <v>1.62</v>
+        <v>1.42</v>
       </c>
       <c r="M131" t="inlineStr">
         <is>
@@ -12472,7 +12472,7 @@
         </is>
       </c>
       <c r="N131" t="n">
-        <v>3.2</v>
+        <v>3.39</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -12480,7 +12480,7 @@
         </is>
       </c>
       <c r="P131" t="n">
-        <v>3.21</v>
+        <v>3.83</v>
       </c>
       <c r="Q131" t="inlineStr">
         <is>
@@ -12488,7 +12488,7 @@
         </is>
       </c>
       <c r="R131" t="n">
-        <v>4.24</v>
+        <v>4.81</v>
       </c>
       <c r="S131" t="inlineStr">
         <is>
@@ -12496,16 +12496,16 @@
         </is>
       </c>
       <c r="T131" t="n">
-        <v>5.62</v>
+        <v>7.25</v>
       </c>
       <c r="U131" t="inlineStr">
         <is>
-          <t>27/10/2023 14:51</t>
+          <t>27/10/2023 14:53</t>
         </is>
       </c>
       <c r="V131" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-bdin-vidin/W25apBIf/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-marek/WMyC61Zd/</t>
         </is>
       </c>
     </row>
@@ -12533,22 +12533,22 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>CSKA 1948 Sofia II</t>
         </is>
       </c>
       <c r="G132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>Septemvri Sofia</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="I132" t="n">
         <v>0</v>
       </c>
       <c r="J132" t="n">
-        <v>3.35</v>
+        <v>1.46</v>
       </c>
       <c r="K132" t="inlineStr">
         <is>
@@ -12556,15 +12556,15 @@
         </is>
       </c>
       <c r="L132" t="n">
-        <v>3.78</v>
+        <v>1.51</v>
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>27/10/2023 14:50</t>
+          <t>27/10/2023 14:53</t>
         </is>
       </c>
       <c r="N132" t="n">
-        <v>2.93</v>
+        <v>3.67</v>
       </c>
       <c r="O132" t="inlineStr">
         <is>
@@ -12572,15 +12572,15 @@
         </is>
       </c>
       <c r="P132" t="n">
-        <v>3.4</v>
+        <v>3.64</v>
       </c>
       <c r="Q132" t="inlineStr">
         <is>
-          <t>27/10/2023 14:50</t>
+          <t>27/10/2023 14:53</t>
         </is>
       </c>
       <c r="R132" t="n">
-        <v>1.95</v>
+        <v>5.19</v>
       </c>
       <c r="S132" t="inlineStr">
         <is>
@@ -12588,16 +12588,16 @@
         </is>
       </c>
       <c r="T132" t="n">
-        <v>1.83</v>
+        <v>5.9</v>
       </c>
       <c r="U132" t="inlineStr">
         <is>
-          <t>27/10/2023 14:50</t>
+          <t>27/10/2023 14:53</t>
         </is>
       </c>
       <c r="V132" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-septemvri-sofia/ADzG5Ll3/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/cska-1948-sofia-chernomorets-1919/Ag43qVX0/</t>
         </is>
       </c>
     </row>
@@ -12625,22 +12625,22 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Ludogorets II</t>
         </is>
       </c>
       <c r="G133" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Yantra Gabrovo</t>
+          <t>Belasitsa</t>
         </is>
       </c>
       <c r="I133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J133" t="n">
-        <v>2.52</v>
+        <v>1.68</v>
       </c>
       <c r="K133" t="inlineStr">
         <is>
@@ -12648,15 +12648,15 @@
         </is>
       </c>
       <c r="L133" t="n">
-        <v>3.05</v>
+        <v>1.6</v>
       </c>
       <c r="M133" t="inlineStr">
         <is>
-          <t>27/10/2023 14:49</t>
+          <t>27/10/2023 13:03</t>
         </is>
       </c>
       <c r="N133" t="n">
-        <v>2.7</v>
+        <v>3.24</v>
       </c>
       <c r="O133" t="inlineStr">
         <is>
@@ -12664,15 +12664,15 @@
         </is>
       </c>
       <c r="P133" t="n">
-        <v>2.51</v>
+        <v>3.51</v>
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>27/10/2023 14:46</t>
+          <t>27/10/2023 13:41</t>
         </is>
       </c>
       <c r="R133" t="n">
-        <v>2.64</v>
+        <v>4.05</v>
       </c>
       <c r="S133" t="inlineStr">
         <is>
@@ -12680,16 +12680,16 @@
         </is>
       </c>
       <c r="T133" t="n">
-        <v>2.64</v>
+        <v>5.13</v>
       </c>
       <c r="U133" t="inlineStr">
         <is>
-          <t>27/10/2023 14:49</t>
+          <t>27/10/2023 13:03</t>
         </is>
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-yantra-gabrovo/SUb8rkm7/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-belasitsa-petrich/xt6eoi3l/</t>
         </is>
       </c>
     </row>
@@ -13361,22 +13361,22 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>Spartak Varna</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="G141" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>Ludogorets II</t>
+          <t>Litex Lovech</t>
         </is>
       </c>
       <c r="I141" t="n">
         <v>0</v>
       </c>
       <c r="J141" t="n">
-        <v>1.38</v>
+        <v>2</v>
       </c>
       <c r="K141" t="inlineStr">
         <is>
@@ -13384,15 +13384,15 @@
         </is>
       </c>
       <c r="L141" t="n">
-        <v>1.22</v>
+        <v>2.01</v>
       </c>
       <c r="M141" t="inlineStr">
         <is>
-          <t>07/11/2023 13:26</t>
+          <t>07/11/2023 13:28</t>
         </is>
       </c>
       <c r="N141" t="n">
-        <v>4.19</v>
+        <v>3.08</v>
       </c>
       <c r="O141" t="inlineStr">
         <is>
@@ -13400,15 +13400,15 @@
         </is>
       </c>
       <c r="P141" t="n">
-        <v>5.28</v>
+        <v>3.13</v>
       </c>
       <c r="Q141" t="inlineStr">
         <is>
-          <t>07/11/2023 13:26</t>
+          <t>07/11/2023 13:28</t>
         </is>
       </c>
       <c r="R141" t="n">
-        <v>6.34</v>
+        <v>3.37</v>
       </c>
       <c r="S141" t="inlineStr">
         <is>
@@ -13416,16 +13416,16 @@
         </is>
       </c>
       <c r="T141" t="n">
-        <v>10.71</v>
+        <v>3.47</v>
       </c>
       <c r="U141" t="inlineStr">
         <is>
-          <t>07/11/2023 13:26</t>
+          <t>07/11/2023 13:28</t>
         </is>
       </c>
       <c r="V141" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-varna-ludogorets/GWQUajIs/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-litex-lovech/p6VYbAXm/</t>
         </is>
       </c>
     </row>
@@ -13453,22 +13453,22 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Spartak Varna</t>
         </is>
       </c>
       <c r="G142" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>Litex Lovech</t>
+          <t>Ludogorets II</t>
         </is>
       </c>
       <c r="I142" t="n">
         <v>0</v>
       </c>
       <c r="J142" t="n">
-        <v>2</v>
+        <v>1.38</v>
       </c>
       <c r="K142" t="inlineStr">
         <is>
@@ -13476,15 +13476,15 @@
         </is>
       </c>
       <c r="L142" t="n">
-        <v>2.01</v>
+        <v>1.22</v>
       </c>
       <c r="M142" t="inlineStr">
         <is>
-          <t>07/11/2023 13:28</t>
+          <t>07/11/2023 13:26</t>
         </is>
       </c>
       <c r="N142" t="n">
-        <v>3.08</v>
+        <v>4.19</v>
       </c>
       <c r="O142" t="inlineStr">
         <is>
@@ -13492,15 +13492,15 @@
         </is>
       </c>
       <c r="P142" t="n">
-        <v>3.13</v>
+        <v>5.28</v>
       </c>
       <c r="Q142" t="inlineStr">
         <is>
-          <t>07/11/2023 13:28</t>
+          <t>07/11/2023 13:26</t>
         </is>
       </c>
       <c r="R142" t="n">
-        <v>3.37</v>
+        <v>6.34</v>
       </c>
       <c r="S142" t="inlineStr">
         <is>
@@ -13508,16 +13508,16 @@
         </is>
       </c>
       <c r="T142" t="n">
-        <v>3.47</v>
+        <v>10.71</v>
       </c>
       <c r="U142" t="inlineStr">
         <is>
-          <t>07/11/2023 13:28</t>
+          <t>07/11/2023 13:26</t>
         </is>
       </c>
       <c r="V142" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/maritsa-plovdiv-litex-lovech/p6VYbAXm/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-varna-ludogorets/GWQUajIs/</t>
         </is>
       </c>
     </row>
@@ -13637,7 +13637,7 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>Ludogorets II</t>
+          <t>Yantra Gabrovo</t>
         </is>
       </c>
       <c r="G144" t="n">
@@ -13645,14 +13645,14 @@
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>Maritsa Plovdiv</t>
+          <t>Chernomorets 1919</t>
         </is>
       </c>
       <c r="I144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J144" t="n">
-        <v>1.73</v>
+        <v>1.67</v>
       </c>
       <c r="K144" t="inlineStr">
         <is>
@@ -13660,15 +13660,15 @@
         </is>
       </c>
       <c r="L144" t="n">
-        <v>1.48</v>
+        <v>1.6</v>
       </c>
       <c r="M144" t="inlineStr">
         <is>
-          <t>11/11/2023 13:27</t>
+          <t>11/11/2023 13:15</t>
         </is>
       </c>
       <c r="N144" t="n">
-        <v>3.45</v>
+        <v>3.3</v>
       </c>
       <c r="O144" t="inlineStr">
         <is>
@@ -13676,15 +13676,15 @@
         </is>
       </c>
       <c r="P144" t="n">
-        <v>3.85</v>
+        <v>3.33</v>
       </c>
       <c r="Q144" t="inlineStr">
         <is>
-          <t>11/11/2023 13:27</t>
+          <t>11/11/2023 13:15</t>
         </is>
       </c>
       <c r="R144" t="n">
-        <v>3.92</v>
+        <v>4.55</v>
       </c>
       <c r="S144" t="inlineStr">
         <is>
@@ -13692,16 +13692,16 @@
         </is>
       </c>
       <c r="T144" t="n">
-        <v>5.95</v>
+        <v>5.56</v>
       </c>
       <c r="U144" t="inlineStr">
         <is>
-          <t>11/11/2023 13:27</t>
+          <t>11/11/2023 13:15</t>
         </is>
       </c>
       <c r="V144" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-maritsa-plovdiv/l0D0D9ns/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/yantra-gabrovo-chernomorets-1919/hhAH9Ro6/</t>
         </is>
       </c>
     </row>
@@ -13729,7 +13729,7 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>Yantra Gabrovo</t>
+          <t>Ludogorets II</t>
         </is>
       </c>
       <c r="G145" t="n">
@@ -13737,14 +13737,14 @@
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>Chernomorets 1919</t>
+          <t>Maritsa Plovdiv</t>
         </is>
       </c>
       <c r="I145" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J145" t="n">
-        <v>1.67</v>
+        <v>1.73</v>
       </c>
       <c r="K145" t="inlineStr">
         <is>
@@ -13752,15 +13752,15 @@
         </is>
       </c>
       <c r="L145" t="n">
-        <v>1.6</v>
+        <v>1.48</v>
       </c>
       <c r="M145" t="inlineStr">
         <is>
-          <t>11/11/2023 13:15</t>
+          <t>11/11/2023 13:27</t>
         </is>
       </c>
       <c r="N145" t="n">
-        <v>3.3</v>
+        <v>3.45</v>
       </c>
       <c r="O145" t="inlineStr">
         <is>
@@ -13768,15 +13768,15 @@
         </is>
       </c>
       <c r="P145" t="n">
-        <v>3.33</v>
+        <v>3.85</v>
       </c>
       <c r="Q145" t="inlineStr">
         <is>
-          <t>11/11/2023 13:15</t>
+          <t>11/11/2023 13:27</t>
         </is>
       </c>
       <c r="R145" t="n">
-        <v>4.55</v>
+        <v>3.92</v>
       </c>
       <c r="S145" t="inlineStr">
         <is>
@@ -13784,16 +13784,16 @@
         </is>
       </c>
       <c r="T145" t="n">
-        <v>5.56</v>
+        <v>5.95</v>
       </c>
       <c r="U145" t="inlineStr">
         <is>
-          <t>11/11/2023 13:15</t>
+          <t>11/11/2023 13:27</t>
         </is>
       </c>
       <c r="V145" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/yantra-gabrovo-chernomorets-1919/hhAH9Ro6/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/ludogorets-maritsa-plovdiv/l0D0D9ns/</t>
         </is>
       </c>
     </row>
@@ -13821,22 +13821,22 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>Svoge</t>
+          <t>Chernomorets Balchik</t>
         </is>
       </c>
       <c r="G146" t="n">
+        <v>0</v>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Septemvri Sofia</t>
+        </is>
+      </c>
+      <c r="I146" t="n">
         <v>2</v>
       </c>
-      <c r="H146" t="inlineStr">
-        <is>
-          <t>Bdin Vidin</t>
-        </is>
-      </c>
-      <c r="I146" t="n">
-        <v>0</v>
-      </c>
       <c r="J146" t="n">
-        <v>1.64</v>
+        <v>5.09</v>
       </c>
       <c r="K146" t="inlineStr">
         <is>
@@ -13844,48 +13844,48 @@
         </is>
       </c>
       <c r="L146" t="n">
+        <v>6.24</v>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>12/11/2023 13:15</t>
+        </is>
+      </c>
+      <c r="N146" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="O146" t="inlineStr">
+        <is>
+          <t>12/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="P146" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="Q146" t="inlineStr">
+        <is>
+          <t>12/11/2023 13:15</t>
+        </is>
+      </c>
+      <c r="R146" t="n">
         <v>1.56</v>
       </c>
-      <c r="M146" t="inlineStr">
-        <is>
-          <t>12/11/2023 13:28</t>
-        </is>
-      </c>
-      <c r="N146" t="n">
-        <v>3.34</v>
-      </c>
-      <c r="O146" t="inlineStr">
+      <c r="S146" t="inlineStr">
         <is>
           <t>12/11/2023 02:42</t>
         </is>
       </c>
-      <c r="P146" t="n">
-        <v>3.44</v>
-      </c>
-      <c r="Q146" t="inlineStr">
-        <is>
-          <t>12/11/2023 13:28</t>
-        </is>
-      </c>
-      <c r="R146" t="n">
-        <v>4.93</v>
-      </c>
-      <c r="S146" t="inlineStr">
-        <is>
-          <t>12/11/2023 02:42</t>
-        </is>
-      </c>
       <c r="T146" t="n">
-        <v>5.77</v>
+        <v>1.46</v>
       </c>
       <c r="U146" t="inlineStr">
         <is>
-          <t>12/11/2023 13:28</t>
+          <t>12/11/2023 13:15</t>
         </is>
       </c>
       <c r="V146" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-bdin-vidin/OI5DA7Wa/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-septemvri-sofia/hURUIVOJ/</t>
         </is>
       </c>
     </row>
@@ -13913,22 +13913,22 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>Chernomorets Balchik</t>
+          <t>Litex Lovech</t>
         </is>
       </c>
       <c r="G147" t="n">
+        <v>1</v>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Dunav Ruse</t>
+        </is>
+      </c>
+      <c r="I147" t="n">
         <v>0</v>
       </c>
-      <c r="H147" t="inlineStr">
-        <is>
-          <t>Septemvri Sofia</t>
-        </is>
-      </c>
-      <c r="I147" t="n">
-        <v>2</v>
-      </c>
       <c r="J147" t="n">
-        <v>5.09</v>
+        <v>2.62</v>
       </c>
       <c r="K147" t="inlineStr">
         <is>
@@ -13936,48 +13936,48 @@
         </is>
       </c>
       <c r="L147" t="n">
-        <v>6.24</v>
+        <v>2.06</v>
       </c>
       <c r="M147" t="inlineStr">
         <is>
-          <t>12/11/2023 13:15</t>
+          <t>12/11/2023 13:22</t>
         </is>
       </c>
       <c r="N147" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>12/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="P147" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>12/11/2023 13:22</t>
+        </is>
+      </c>
+      <c r="R147" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="S147" t="inlineStr">
+        <is>
+          <t>12/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="T147" t="n">
         <v>3.54</v>
       </c>
-      <c r="O147" t="inlineStr">
-        <is>
-          <t>12/11/2023 02:42</t>
-        </is>
-      </c>
-      <c r="P147" t="n">
-        <v>3.84</v>
-      </c>
-      <c r="Q147" t="inlineStr">
-        <is>
-          <t>12/11/2023 13:15</t>
-        </is>
-      </c>
-      <c r="R147" t="n">
-        <v>1.56</v>
-      </c>
-      <c r="S147" t="inlineStr">
-        <is>
-          <t>12/11/2023 02:42</t>
-        </is>
-      </c>
-      <c r="T147" t="n">
-        <v>1.46</v>
-      </c>
       <c r="U147" t="inlineStr">
         <is>
-          <t>12/11/2023 13:15</t>
+          <t>12/11/2023 13:22</t>
         </is>
       </c>
       <c r="V147" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/chernomorets-balchik-septemvri-sofia/hURUIVOJ/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/litex-lovech-dunav-ruse/WKQYHkvQ/</t>
         </is>
       </c>
     </row>
@@ -14005,22 +14005,22 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>Litex Lovech</t>
+          <t>Spartak Pleven</t>
         </is>
       </c>
       <c r="G148" t="n">
+        <v>2</v>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Spartak Varna</t>
+        </is>
+      </c>
+      <c r="I148" t="n">
         <v>1</v>
       </c>
-      <c r="H148" t="inlineStr">
-        <is>
-          <t>Dunav Ruse</t>
-        </is>
-      </c>
-      <c r="I148" t="n">
-        <v>0</v>
-      </c>
       <c r="J148" t="n">
-        <v>2.62</v>
+        <v>4.82</v>
       </c>
       <c r="K148" t="inlineStr">
         <is>
@@ -14028,15 +14028,15 @@
         </is>
       </c>
       <c r="L148" t="n">
-        <v>2.06</v>
+        <v>5.52</v>
       </c>
       <c r="M148" t="inlineStr">
         <is>
-          <t>12/11/2023 13:22</t>
+          <t>12/11/2023 12:36</t>
         </is>
       </c>
       <c r="N148" t="n">
-        <v>2.74</v>
+        <v>3.49</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -14044,15 +14044,15 @@
         </is>
       </c>
       <c r="P148" t="n">
-        <v>2.96</v>
+        <v>3.67</v>
       </c>
       <c r="Q148" t="inlineStr">
         <is>
-          <t>12/11/2023 13:22</t>
+          <t>12/11/2023 12:36</t>
         </is>
       </c>
       <c r="R148" t="n">
-        <v>2.75</v>
+        <v>1.59</v>
       </c>
       <c r="S148" t="inlineStr">
         <is>
@@ -14060,16 +14060,16 @@
         </is>
       </c>
       <c r="T148" t="n">
-        <v>3.54</v>
+        <v>1.53</v>
       </c>
       <c r="U148" t="inlineStr">
         <is>
-          <t>12/11/2023 13:22</t>
+          <t>12/11/2023 12:36</t>
         </is>
       </c>
       <c r="V148" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/litex-lovech-dunav-ruse/WKQYHkvQ/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-spartak-varna/23H4CT1m/</t>
         </is>
       </c>
     </row>
@@ -14097,22 +14097,22 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>Spartak Pleven</t>
+          <t>Strumska Slava</t>
         </is>
       </c>
       <c r="G149" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>Spartak Varna</t>
+          <t>Marek</t>
         </is>
       </c>
       <c r="I149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J149" t="n">
-        <v>4.82</v>
+        <v>2.09</v>
       </c>
       <c r="K149" t="inlineStr">
         <is>
@@ -14120,15 +14120,15 @@
         </is>
       </c>
       <c r="L149" t="n">
-        <v>5.52</v>
+        <v>1.8</v>
       </c>
       <c r="M149" t="inlineStr">
         <is>
-          <t>12/11/2023 12:36</t>
+          <t>12/11/2023 13:06</t>
         </is>
       </c>
       <c r="N149" t="n">
-        <v>3.49</v>
+        <v>2.93</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -14136,15 +14136,15 @@
         </is>
       </c>
       <c r="P149" t="n">
-        <v>3.67</v>
+        <v>3.09</v>
       </c>
       <c r="Q149" t="inlineStr">
         <is>
-          <t>12/11/2023 12:36</t>
+          <t>12/11/2023 13:06</t>
         </is>
       </c>
       <c r="R149" t="n">
-        <v>1.59</v>
+        <v>3.33</v>
       </c>
       <c r="S149" t="inlineStr">
         <is>
@@ -14152,16 +14152,16 @@
         </is>
       </c>
       <c r="T149" t="n">
-        <v>1.53</v>
+        <v>4.41</v>
       </c>
       <c r="U149" t="inlineStr">
         <is>
-          <t>12/11/2023 12:36</t>
+          <t>12/11/2023 13:06</t>
         </is>
       </c>
       <c r="V149" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/spartak-pleven-spartak-varna/23H4CT1m/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-marek/EoNkeSWC/</t>
         </is>
       </c>
     </row>
@@ -14189,22 +14189,22 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>Strumska Slava</t>
+          <t>Svoge</t>
         </is>
       </c>
       <c r="G150" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>Marek</t>
+          <t>Bdin Vidin</t>
         </is>
       </c>
       <c r="I150" t="n">
         <v>0</v>
       </c>
       <c r="J150" t="n">
-        <v>2.09</v>
+        <v>1.64</v>
       </c>
       <c r="K150" t="inlineStr">
         <is>
@@ -14212,15 +14212,15 @@
         </is>
       </c>
       <c r="L150" t="n">
-        <v>1.8</v>
+        <v>1.56</v>
       </c>
       <c r="M150" t="inlineStr">
         <is>
-          <t>12/11/2023 13:06</t>
+          <t>12/11/2023 13:28</t>
         </is>
       </c>
       <c r="N150" t="n">
-        <v>2.93</v>
+        <v>3.34</v>
       </c>
       <c r="O150" t="inlineStr">
         <is>
@@ -14228,15 +14228,15 @@
         </is>
       </c>
       <c r="P150" t="n">
-        <v>3.09</v>
+        <v>3.44</v>
       </c>
       <c r="Q150" t="inlineStr">
         <is>
-          <t>12/11/2023 13:06</t>
+          <t>12/11/2023 13:28</t>
         </is>
       </c>
       <c r="R150" t="n">
-        <v>3.33</v>
+        <v>4.93</v>
       </c>
       <c r="S150" t="inlineStr">
         <is>
@@ -14244,16 +14244,16 @@
         </is>
       </c>
       <c r="T150" t="n">
-        <v>4.41</v>
+        <v>5.77</v>
       </c>
       <c r="U150" t="inlineStr">
         <is>
-          <t>12/11/2023 13:06</t>
+          <t>12/11/2023 13:28</t>
         </is>
       </c>
       <c r="V150" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/strumska-slava-marek/EoNkeSWC/</t>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/svoge-bdin-vidin/OI5DA7Wa/</t>
         </is>
       </c>
     </row>
@@ -15082,6 +15082,98 @@
       <c r="V159" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/marek-chernomorets-1919/Wr9L8o1C/</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>bulgaria</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>vtora-liga</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E160" s="2" t="n">
+        <v>45261.54166666666</v>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Dobrudzha</t>
+        </is>
+      </c>
+      <c r="G160" t="n">
+        <v>0</v>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>Litex Lovech</t>
+        </is>
+      </c>
+      <c r="I160" t="n">
+        <v>1</v>
+      </c>
+      <c r="J160" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>01/12/2023 01:13</t>
+        </is>
+      </c>
+      <c r="L160" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>01/12/2023 12:03</t>
+        </is>
+      </c>
+      <c r="N160" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="O160" t="inlineStr">
+        <is>
+          <t>01/12/2023 01:13</t>
+        </is>
+      </c>
+      <c r="P160" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="Q160" t="inlineStr">
+        <is>
+          <t>01/12/2023 12:03</t>
+        </is>
+      </c>
+      <c r="R160" t="n">
+        <v>7.49</v>
+      </c>
+      <c r="S160" t="inlineStr">
+        <is>
+          <t>01/12/2023 01:13</t>
+        </is>
+      </c>
+      <c r="T160" t="n">
+        <v>10.29</v>
+      </c>
+      <c r="U160" t="inlineStr">
+        <is>
+          <t>01/12/2023 12:03</t>
+        </is>
+      </c>
+      <c r="V160" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/bulgaria/vtora-liga/dobrudzha-litex-lovech/0xx7Kr0O/</t>
         </is>
       </c>
     </row>

</xml_diff>